<commit_message>
adding category and factor explanations
</commit_message>
<xml_diff>
--- a/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
+++ b/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Library/CloudStorage/OneDrive-Personal/Revenue Streams/Field Factors/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Downloads/rsc-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0F3501F-CF08-BF4E-971E-274ACD101B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2C9306-E1D5-9D44-A323-613055F73A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
     <sheet name="Inputs" sheetId="2" r:id="rId2"/>
     <sheet name="Weights" sheetId="3" r:id="rId3"/>
     <sheet name="Scoring" sheetId="4" r:id="rId4"/>
-    <sheet name="Snippets" sheetId="5" r:id="rId5"/>
-    <sheet name="Results" sheetId="6" r:id="rId6"/>
+    <sheet name="Categories" sheetId="7" r:id="rId5"/>
+    <sheet name="Factors" sheetId="8" r:id="rId6"/>
+    <sheet name="Snippets" sheetId="5" r:id="rId7"/>
+    <sheet name="Results" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="130">
   <si>
     <t>Section</t>
   </si>
@@ -241,6 +243,219 @@
   </si>
   <si>
     <t>Weaknesses &amp; Threats</t>
+  </si>
+  <si>
+    <t>factor_name</t>
+  </si>
+  <si>
+    <t>factor_id</t>
+  </si>
+  <si>
+    <t>category_name</t>
+  </si>
+  <si>
+    <t>factor_description</t>
+  </si>
+  <si>
+    <t>left_label</t>
+  </si>
+  <si>
+    <t>right_label</t>
+  </si>
+  <si>
+    <t>customer_service_sales</t>
+  </si>
+  <si>
+    <t>Customer Facing Skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How confident and experienced are you when it comes to engaging with customers — answering questions, handling service issues, pitching your offerings, and closing a sale (whether in person, by email, or over social media)? </t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>marketing</t>
+  </si>
+  <si>
+    <t>Do you have experience promoting your business through digital and print marketing? This could include things like social media posts, email campaigns, flyers or other printed materials, pitches to media outlets, writing captions, taking great photos, or running paid ads (like on Meta or Google) to help increase visibility and drive sales.</t>
+  </si>
+  <si>
+    <t>personal_connections</t>
+  </si>
+  <si>
+    <t>Networks</t>
+  </si>
+  <si>
+    <t>Do you belong to neighborhood organizations, faith groups, clubs, or social circles where you can share your business, gather support, or spread the word?</t>
+  </si>
+  <si>
+    <t>professional_network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you connected with other local businesses, market organizations, or industry groups that could support, promote, or collaborate with your flower business? </t>
+  </si>
+  <si>
+    <t>proximity_to_customers</t>
+  </si>
+  <si>
+    <t>Location and Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Is your farm located near one or more population centers, wedding/event venues, agri-tourism destinations, or established farmers markets? Or are you more remote, requiring longer travel times for you and/or your customers?</t>
+  </si>
+  <si>
+    <t>Aesthetic &amp; Experiential Appeal</t>
+  </si>
+  <si>
+    <t>aesthetic_experiential_appeal</t>
+  </si>
+  <si>
+    <t>Does your farm offer a visually appealing or memorable experience — such as scenic views, rustic buildings, flower fields, or friendly animals — that could enhance on-farm events or help entice customers to visit?</t>
+  </si>
+  <si>
+    <t>customer_friendly_amenities</t>
+  </si>
+  <si>
+    <t>Do you have infrastructure in place to welcome and support visitors, like parking, restrooms, shaded seating, or accessible paths?</t>
+  </si>
+  <si>
+    <t>regulatory_freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Are there zoning laws, HOA restrictions, or permitting requirements that could limit your ability to host events, build structures, or sell directly from your farm?</t>
+  </si>
+  <si>
+    <t>high_volume_production</t>
+  </si>
+  <si>
+    <t>Farm Production</t>
+  </si>
+  <si>
+    <t>Can your farm produce a large quantity of flowers? Or are you limited to smaller-scale production due to space, labor, or other constraints?</t>
+  </si>
+  <si>
+    <t>operational_infrastructure</t>
+  </si>
+  <si>
+    <t>Do you have systems and spaces in place to efficiently store, arrange, and transport your flowers — such as refrigeration, workstations, storage areas, and a reliable vehicle suited for moving product at scale?</t>
+  </si>
+  <si>
+    <t>product_diversity</t>
+  </si>
+  <si>
+    <t>Can you grow a wide variety of floral ingredients, including all six Bouquet Blueprint™ categories? Or is your production limited by space, climate, or your preference for focusing on a single crop (or very limited number of crops)?</t>
+  </si>
+  <si>
+    <t>product_predictability</t>
+  </si>
+  <si>
+    <t>Are you able to consistently predict bloom timing and availability? Have you implemented strategies like succession planting to ensure a steady, well-timed supply?</t>
+  </si>
+  <si>
+    <t>schedule_flexibility</t>
+  </si>
+  <si>
+    <t>Time and Money</t>
+  </si>
+  <si>
+    <t>How much control do you have over your time? Can you adjust when you work to align with customer needs — for example, being available for weddings, events, or farmers market hours — or do you have other commitments or personal boundaries that shape when and how you run your farm business?</t>
+  </si>
+  <si>
+    <t>financial_resources</t>
+  </si>
+  <si>
+    <t>Do you have capital available to invest in your business? If not, are you eligible for grants or loans, and do you have experience successfully applying for them?</t>
+  </si>
+  <si>
+    <t>floral_design</t>
+  </si>
+  <si>
+    <t>Design Skills</t>
+  </si>
+  <si>
+    <t>Do you have experience making bouquets and arrangements? Are you comfortable designing in a range of styles — such as rustic, garden-inspired, modern, or minimalist — to suit different customers and occasions? Do you keep up with floral trends and design aesthetics? Do you enjoy experimenting with new techniques, forms, or ingredients?</t>
+  </si>
+  <si>
+    <t>Color Comprehension &amp; Accuracy</t>
+  </si>
+  <si>
+    <t>color_comprehension_accuracy</t>
+  </si>
+  <si>
+    <t>Do you have a strong eye for color — including the ability to recognize undertones, distinguish between warm and cool hues, and build harmonious palettes? Are you able to communicate these nuances to customers?</t>
+  </si>
+  <si>
+    <t>social_personality</t>
+  </si>
+  <si>
+    <t>Personal Attributes</t>
+  </si>
+  <si>
+    <t>Are you introverted, extroverted, or somewhere in between?</t>
+  </si>
+  <si>
+    <t>introverted</t>
+  </si>
+  <si>
+    <t>extroverted</t>
+  </si>
+  <si>
+    <t>Stress &amp; Risk Tolerance</t>
+  </si>
+  <si>
+    <t>stress_risk_tolerance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How well do you handle uncertainty, pressure, or fast-changing circumstances? Do you lean more towards the “no risk/no reward” point of view, or are you more of a “better safe than sorry” person? </t>
+  </si>
+  <si>
+    <t>low tolerance</t>
+  </si>
+  <si>
+    <t>high tolerance</t>
+  </si>
+  <si>
+    <t>Time Management &amp; Organization</t>
+  </si>
+  <si>
+    <t>time_management_organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Are you able to structure your time effectively, stay on top of tasks, and meet deadlines? Can you estimate how long things will take, stay prepared with lists or systems, and keep projects moving forward in a timely way?</t>
+  </si>
+  <si>
+    <t>not time effective</t>
+  </si>
+  <si>
+    <t>very time effective</t>
+  </si>
+  <si>
+    <t>category_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How you connect with customers — and how often — can vary widely between different sales channels. This section helps you reflect on your comfort and strengths when it comes to engaging with customers, promoting your business, and making the sale.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farming can feel isolating at times — but strong networks can open doors, spread the word, and make the work more sustainable. The connections you already have (or are willing to build) can shape how easily you access new opportunities, especially in revenue streams that thrive on community reach and local engagement. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where you grow — and who’s around you — shapes everything from market access to hosting customers at the farm. Understanding the strengths and limitations of your location will help you make strategic decisions about which sales channels are most feasible and profitable. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your farm’s growing conditions, infrastructure, and output shape what (and how much of it) you can offer, and how consistently you can offer it. This section helps you assess how well your space supports the type, volume, and timing of production that different revenue streams may require. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your available time and financial capacity shape how quickly you can grow—and how much you can take on. Getting honest about both helps you choose a business model that aligns with your real-life bandwidth and budget. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some revenue streams—like retail bouquets, weddings, or workshops—depend heavily on strong floral design. This section helps you assess whether those design-focused paths align with your current strengths, your creative interests, or your willingness to grow. </t>
+  </si>
+  <si>
+    <t>Your natural tendencies, preferences, and decision-making style shape how you run your business. Knowing yourself helps you build a business that feels sustainable and enjoyable, not draining.</t>
   </si>
 </sst>
 </file>
@@ -250,7 +465,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +494,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -329,7 +557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -339,9 +567,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -371,9 +596,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -911,1179 +1149,1179 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8">
-        <v>2</v>
-      </c>
-      <c r="E2" s="8">
-        <v>4</v>
-      </c>
-      <c r="F2" s="8">
-        <v>3</v>
-      </c>
-      <c r="G2" s="8">
-        <v>3</v>
-      </c>
-      <c r="H2" s="8">
-        <v>2</v>
-      </c>
-      <c r="I2" s="8">
-        <v>2</v>
-      </c>
-      <c r="J2" s="8">
-        <v>1</v>
-      </c>
-      <c r="K2" s="8">
-        <v>2</v>
-      </c>
-      <c r="L2" s="8">
-        <v>2</v>
-      </c>
-      <c r="M2" s="8">
-        <v>5</v>
-      </c>
-      <c r="N2" s="8">
-        <v>3</v>
-      </c>
-      <c r="O2" s="8">
-        <v>4</v>
-      </c>
-      <c r="P2" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="8">
-        <v>4</v>
-      </c>
-      <c r="R2" s="8">
-        <v>4</v>
-      </c>
-      <c r="S2" s="8">
+      <c r="B2" s="7">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7">
+        <v>3</v>
+      </c>
+      <c r="H2" s="7">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7">
+        <v>2</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7">
+        <v>2</v>
+      </c>
+      <c r="L2" s="7">
+        <v>2</v>
+      </c>
+      <c r="M2" s="7">
+        <v>5</v>
+      </c>
+      <c r="N2" s="7">
+        <v>3</v>
+      </c>
+      <c r="O2" s="7">
+        <v>4</v>
+      </c>
+      <c r="P2" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>4</v>
+      </c>
+      <c r="R2" s="7">
+        <v>4</v>
+      </c>
+      <c r="S2" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8">
-        <v>2</v>
-      </c>
-      <c r="C3" s="8">
-        <v>5</v>
-      </c>
-      <c r="D3" s="8">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8">
-        <v>5</v>
-      </c>
-      <c r="F3" s="8">
-        <v>5</v>
-      </c>
-      <c r="G3" s="8">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="J3" s="8">
-        <v>2</v>
-      </c>
-      <c r="K3" s="8">
-        <v>3</v>
-      </c>
-      <c r="L3" s="8">
-        <v>3</v>
-      </c>
-      <c r="M3" s="8">
-        <v>5</v>
-      </c>
-      <c r="N3" s="8">
-        <v>5</v>
-      </c>
-      <c r="O3" s="8">
-        <v>4</v>
-      </c>
-      <c r="P3" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="8">
-        <v>5</v>
-      </c>
-      <c r="R3" s="8">
-        <v>5</v>
-      </c>
-      <c r="S3" s="8">
+      <c r="B3" s="7">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>5</v>
+      </c>
+      <c r="D3" s="7">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7">
+        <v>5</v>
+      </c>
+      <c r="F3" s="7">
+        <v>5</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>2</v>
+      </c>
+      <c r="K3" s="7">
+        <v>3</v>
+      </c>
+      <c r="L3" s="7">
+        <v>3</v>
+      </c>
+      <c r="M3" s="7">
+        <v>5</v>
+      </c>
+      <c r="N3" s="7">
+        <v>5</v>
+      </c>
+      <c r="O3" s="7">
+        <v>4</v>
+      </c>
+      <c r="P3" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>5</v>
+      </c>
+      <c r="R3" s="7">
+        <v>5</v>
+      </c>
+      <c r="S3" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8">
-        <v>4</v>
-      </c>
-      <c r="D4" s="8">
-        <v>4</v>
-      </c>
-      <c r="E4" s="8">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8">
-        <v>2</v>
-      </c>
-      <c r="G4" s="8">
-        <v>1</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8">
-        <v>1</v>
-      </c>
-      <c r="J4" s="8">
-        <v>1</v>
-      </c>
-      <c r="K4" s="8">
-        <v>1</v>
-      </c>
-      <c r="L4" s="8">
-        <v>1</v>
-      </c>
-      <c r="M4" s="8">
-        <v>3</v>
-      </c>
-      <c r="N4" s="8">
-        <v>3</v>
-      </c>
-      <c r="O4" s="8">
-        <v>1</v>
-      </c>
-      <c r="P4" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>3</v>
-      </c>
-      <c r="R4" s="8">
-        <v>3</v>
-      </c>
-      <c r="S4" s="8">
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7">
+        <v>4</v>
+      </c>
+      <c r="E4" s="7">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>3</v>
+      </c>
+      <c r="N4" s="7">
+        <v>3</v>
+      </c>
+      <c r="O4" s="7">
+        <v>1</v>
+      </c>
+      <c r="P4" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>3</v>
+      </c>
+      <c r="R4" s="7">
+        <v>3</v>
+      </c>
+      <c r="S4" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8">
-        <v>1</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1</v>
-      </c>
-      <c r="J5" s="8">
-        <v>3</v>
-      </c>
-      <c r="K5" s="8">
-        <v>4</v>
-      </c>
-      <c r="L5" s="8">
-        <v>4</v>
-      </c>
-      <c r="M5" s="8">
-        <v>1</v>
-      </c>
-      <c r="N5" s="8">
-        <v>1</v>
-      </c>
-      <c r="O5" s="8">
-        <v>4</v>
-      </c>
-      <c r="P5" s="8">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>3</v>
-      </c>
-      <c r="R5" s="8">
-        <v>3</v>
-      </c>
-      <c r="S5" s="8">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>3</v>
+      </c>
+      <c r="K5" s="7">
+        <v>4</v>
+      </c>
+      <c r="L5" s="7">
+        <v>4</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1</v>
+      </c>
+      <c r="N5" s="7">
+        <v>1</v>
+      </c>
+      <c r="O5" s="7">
+        <v>4</v>
+      </c>
+      <c r="P5" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>3</v>
+      </c>
+      <c r="R5" s="7">
+        <v>3</v>
+      </c>
+      <c r="S5" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="8">
-        <v>4</v>
-      </c>
-      <c r="C6" s="8">
-        <v>4</v>
-      </c>
-      <c r="D6" s="8">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8">
-        <v>4</v>
-      </c>
-      <c r="F6" s="8">
-        <v>3</v>
-      </c>
-      <c r="G6" s="8">
-        <v>3</v>
-      </c>
-      <c r="H6" s="8">
-        <v>3</v>
-      </c>
-      <c r="I6" s="8">
-        <v>3</v>
-      </c>
-      <c r="J6" s="8">
-        <v>3</v>
-      </c>
-      <c r="K6" s="8">
-        <v>4</v>
-      </c>
-      <c r="L6" s="8">
-        <v>5</v>
-      </c>
-      <c r="M6" s="8">
-        <v>3</v>
-      </c>
-      <c r="N6" s="8">
-        <v>3</v>
-      </c>
-      <c r="O6" s="8">
-        <v>3</v>
-      </c>
-      <c r="P6" s="8">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="8">
-        <v>3</v>
-      </c>
-      <c r="R6" s="8">
-        <v>3</v>
-      </c>
-      <c r="S6" s="8">
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7">
+        <v>4</v>
+      </c>
+      <c r="F6" s="7">
+        <v>3</v>
+      </c>
+      <c r="G6" s="7">
+        <v>3</v>
+      </c>
+      <c r="H6" s="7">
+        <v>3</v>
+      </c>
+      <c r="I6" s="7">
+        <v>3</v>
+      </c>
+      <c r="J6" s="7">
+        <v>3</v>
+      </c>
+      <c r="K6" s="7">
+        <v>4</v>
+      </c>
+      <c r="L6" s="7">
+        <v>5</v>
+      </c>
+      <c r="M6" s="7">
+        <v>3</v>
+      </c>
+      <c r="N6" s="7">
+        <v>3</v>
+      </c>
+      <c r="O6" s="7">
+        <v>3</v>
+      </c>
+      <c r="P6" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>3</v>
+      </c>
+      <c r="R6" s="7">
+        <v>3</v>
+      </c>
+      <c r="S6" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8">
-        <v>4</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-      <c r="I7" s="8">
-        <v>1</v>
-      </c>
-      <c r="J7" s="8">
-        <v>1</v>
-      </c>
-      <c r="K7" s="8">
-        <v>1</v>
-      </c>
-      <c r="L7" s="8">
-        <v>1</v>
-      </c>
-      <c r="M7" s="8">
-        <v>1</v>
-      </c>
-      <c r="N7" s="8">
-        <v>1</v>
-      </c>
-      <c r="O7" s="8">
-        <v>1</v>
-      </c>
-      <c r="P7" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>4</v>
-      </c>
-      <c r="R7" s="8">
-        <v>4</v>
-      </c>
-      <c r="S7" s="8">
+      <c r="A7" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="7">
+        <v>1</v>
+      </c>
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="7">
+        <v>1</v>
+      </c>
+      <c r="O7" s="7">
+        <v>1</v>
+      </c>
+      <c r="P7" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>4</v>
+      </c>
+      <c r="R7" s="7">
+        <v>4</v>
+      </c>
+      <c r="S7" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="8">
-        <v>3</v>
-      </c>
-      <c r="E8" s="8">
-        <v>2</v>
-      </c>
-      <c r="F8" s="8">
-        <v>2</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="8">
-        <v>1</v>
-      </c>
-      <c r="K8" s="8">
-        <v>1</v>
-      </c>
-      <c r="L8" s="8">
-        <v>1</v>
-      </c>
-      <c r="M8" s="8">
-        <v>1</v>
-      </c>
-      <c r="N8" s="8">
-        <v>2</v>
-      </c>
-      <c r="O8" s="8">
-        <v>1</v>
-      </c>
-      <c r="P8" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>5</v>
-      </c>
-      <c r="R8" s="8">
-        <v>5</v>
-      </c>
-      <c r="S8" s="8">
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>3</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <v>1</v>
+      </c>
+      <c r="K8" s="7">
+        <v>1</v>
+      </c>
+      <c r="L8" s="7">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7">
+        <v>2</v>
+      </c>
+      <c r="O8" s="7">
+        <v>1</v>
+      </c>
+      <c r="P8" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>5</v>
+      </c>
+      <c r="R8" s="7">
+        <v>5</v>
+      </c>
+      <c r="S8" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8">
-        <v>1</v>
-      </c>
-      <c r="C9" s="8">
-        <v>2</v>
-      </c>
-      <c r="D9" s="8">
-        <v>4</v>
-      </c>
-      <c r="E9" s="8">
-        <v>2</v>
-      </c>
-      <c r="F9" s="8">
-        <v>2</v>
-      </c>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="8">
-        <v>1</v>
-      </c>
-      <c r="J9" s="8">
-        <v>1</v>
-      </c>
-      <c r="K9" s="8">
-        <v>1</v>
-      </c>
-      <c r="L9" s="8">
-        <v>1</v>
-      </c>
-      <c r="M9" s="8">
-        <v>1</v>
-      </c>
-      <c r="N9" s="8">
-        <v>2</v>
-      </c>
-      <c r="O9" s="8">
-        <v>1</v>
-      </c>
-      <c r="P9" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="8">
-        <v>5</v>
-      </c>
-      <c r="R9" s="8">
-        <v>5</v>
-      </c>
-      <c r="S9" s="8">
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7">
+        <v>1</v>
+      </c>
+      <c r="L9" s="7">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7">
+        <v>1</v>
+      </c>
+      <c r="N9" s="7">
+        <v>2</v>
+      </c>
+      <c r="O9" s="7">
+        <v>1</v>
+      </c>
+      <c r="P9" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>5</v>
+      </c>
+      <c r="R9" s="7">
+        <v>5</v>
+      </c>
+      <c r="S9" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8">
-        <v>5</v>
-      </c>
-      <c r="C10" s="8">
-        <v>5</v>
-      </c>
-      <c r="D10" s="8">
-        <v>4</v>
-      </c>
-      <c r="E10" s="8">
-        <v>5</v>
-      </c>
-      <c r="F10" s="8">
-        <v>4</v>
-      </c>
-      <c r="G10" s="8">
-        <v>1</v>
-      </c>
-      <c r="H10" s="8">
-        <v>1</v>
-      </c>
-      <c r="I10" s="8">
-        <v>4</v>
-      </c>
-      <c r="J10" s="8">
-        <v>1</v>
-      </c>
-      <c r="K10" s="8">
-        <v>4</v>
-      </c>
-      <c r="L10" s="8">
-        <v>4</v>
-      </c>
-      <c r="M10" s="8">
-        <v>5</v>
-      </c>
-      <c r="N10" s="8">
-        <v>5</v>
-      </c>
-      <c r="O10" s="8">
-        <v>5</v>
-      </c>
-      <c r="P10" s="8">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="8">
-        <v>3</v>
-      </c>
-      <c r="R10" s="8">
-        <v>4</v>
-      </c>
-      <c r="S10" s="8">
+      <c r="B10" s="7">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4</v>
+      </c>
+      <c r="E10" s="7">
+        <v>5</v>
+      </c>
+      <c r="F10" s="7">
+        <v>4</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>4</v>
+      </c>
+      <c r="J10" s="7">
+        <v>1</v>
+      </c>
+      <c r="K10" s="7">
+        <v>4</v>
+      </c>
+      <c r="L10" s="7">
+        <v>4</v>
+      </c>
+      <c r="M10" s="7">
+        <v>5</v>
+      </c>
+      <c r="N10" s="7">
+        <v>5</v>
+      </c>
+      <c r="O10" s="7">
+        <v>5</v>
+      </c>
+      <c r="P10" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>3</v>
+      </c>
+      <c r="R10" s="7">
+        <v>4</v>
+      </c>
+      <c r="S10" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8">
-        <v>3</v>
-      </c>
-      <c r="C11" s="8">
-        <v>3</v>
-      </c>
-      <c r="D11" s="8">
-        <v>3</v>
-      </c>
-      <c r="E11" s="8">
-        <v>3</v>
-      </c>
-      <c r="F11" s="8">
-        <v>3</v>
-      </c>
-      <c r="G11" s="8">
-        <v>2</v>
-      </c>
-      <c r="H11" s="8">
-        <v>5</v>
-      </c>
-      <c r="I11" s="8">
-        <v>5</v>
-      </c>
-      <c r="J11" s="8">
-        <v>3</v>
-      </c>
-      <c r="K11" s="8">
-        <v>1</v>
-      </c>
-      <c r="L11" s="8">
-        <v>1</v>
-      </c>
-      <c r="M11" s="8">
-        <v>3</v>
-      </c>
-      <c r="N11" s="8">
-        <v>2</v>
-      </c>
-      <c r="O11" s="8">
-        <v>2</v>
-      </c>
-      <c r="P11" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="8">
-        <v>4</v>
-      </c>
-      <c r="R11" s="8">
-        <v>2</v>
-      </c>
-      <c r="S11" s="8">
+      <c r="B11" s="7">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7">
+        <v>3</v>
+      </c>
+      <c r="D11" s="7">
+        <v>3</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3</v>
+      </c>
+      <c r="G11" s="7">
+        <v>2</v>
+      </c>
+      <c r="H11" s="7">
+        <v>5</v>
+      </c>
+      <c r="I11" s="7">
+        <v>5</v>
+      </c>
+      <c r="J11" s="7">
+        <v>3</v>
+      </c>
+      <c r="K11" s="7">
+        <v>1</v>
+      </c>
+      <c r="L11" s="7">
+        <v>1</v>
+      </c>
+      <c r="M11" s="7">
+        <v>3</v>
+      </c>
+      <c r="N11" s="7">
+        <v>2</v>
+      </c>
+      <c r="O11" s="7">
+        <v>2</v>
+      </c>
+      <c r="P11" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>4</v>
+      </c>
+      <c r="R11" s="7">
+        <v>2</v>
+      </c>
+      <c r="S11" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="8">
-        <v>5</v>
-      </c>
-      <c r="C12" s="8">
-        <v>3</v>
-      </c>
-      <c r="D12" s="8">
-        <v>2</v>
-      </c>
-      <c r="E12" s="8">
-        <v>3</v>
-      </c>
-      <c r="F12" s="8">
-        <v>2</v>
-      </c>
-      <c r="G12" s="8">
-        <v>4</v>
-      </c>
-      <c r="H12" s="8">
-        <v>5</v>
-      </c>
-      <c r="I12" s="8">
-        <v>5</v>
-      </c>
-      <c r="J12" s="8">
-        <v>3</v>
-      </c>
-      <c r="K12" s="8">
-        <v>3</v>
-      </c>
-      <c r="L12" s="8">
-        <v>2</v>
-      </c>
-      <c r="M12" s="8">
-        <v>5</v>
-      </c>
-      <c r="N12" s="8">
-        <v>4</v>
-      </c>
-      <c r="O12" s="8">
-        <v>5</v>
-      </c>
-      <c r="P12" s="8">
-        <v>4</v>
-      </c>
-      <c r="Q12" s="8">
-        <v>1</v>
-      </c>
-      <c r="R12" s="8">
-        <v>3</v>
-      </c>
-      <c r="S12" s="8">
+      <c r="B12" s="7">
+        <v>5</v>
+      </c>
+      <c r="C12" s="7">
+        <v>3</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
+      <c r="G12" s="7">
+        <v>4</v>
+      </c>
+      <c r="H12" s="7">
+        <v>5</v>
+      </c>
+      <c r="I12" s="7">
+        <v>5</v>
+      </c>
+      <c r="J12" s="7">
+        <v>3</v>
+      </c>
+      <c r="K12" s="7">
+        <v>3</v>
+      </c>
+      <c r="L12" s="7">
+        <v>2</v>
+      </c>
+      <c r="M12" s="7">
+        <v>5</v>
+      </c>
+      <c r="N12" s="7">
+        <v>4</v>
+      </c>
+      <c r="O12" s="7">
+        <v>5</v>
+      </c>
+      <c r="P12" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>1</v>
+      </c>
+      <c r="R12" s="7">
+        <v>3</v>
+      </c>
+      <c r="S12" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8">
-        <v>4</v>
-      </c>
-      <c r="C13" s="8">
-        <v>4</v>
-      </c>
-      <c r="D13" s="8">
-        <v>2</v>
-      </c>
-      <c r="E13" s="8">
-        <v>2</v>
-      </c>
-      <c r="F13" s="8">
-        <v>4</v>
-      </c>
-      <c r="G13" s="8">
-        <v>4</v>
-      </c>
-      <c r="H13" s="8">
-        <v>5</v>
-      </c>
-      <c r="I13" s="8">
-        <v>5</v>
-      </c>
-      <c r="J13" s="8">
-        <v>4</v>
-      </c>
-      <c r="K13" s="8">
-        <v>3</v>
-      </c>
-      <c r="L13" s="8">
-        <v>2</v>
-      </c>
-      <c r="M13" s="8">
-        <v>5</v>
-      </c>
-      <c r="N13" s="8">
-        <v>5</v>
-      </c>
-      <c r="O13" s="8">
-        <v>5</v>
-      </c>
-      <c r="P13" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>3</v>
-      </c>
-      <c r="R13" s="8">
-        <v>3</v>
-      </c>
-      <c r="S13" s="8">
+      <c r="B13" s="7">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7">
+        <v>4</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7">
+        <v>2</v>
+      </c>
+      <c r="F13" s="7">
+        <v>4</v>
+      </c>
+      <c r="G13" s="7">
+        <v>4</v>
+      </c>
+      <c r="H13" s="7">
+        <v>5</v>
+      </c>
+      <c r="I13" s="7">
+        <v>5</v>
+      </c>
+      <c r="J13" s="7">
+        <v>4</v>
+      </c>
+      <c r="K13" s="7">
+        <v>3</v>
+      </c>
+      <c r="L13" s="7">
+        <v>2</v>
+      </c>
+      <c r="M13" s="7">
+        <v>5</v>
+      </c>
+      <c r="N13" s="7">
+        <v>5</v>
+      </c>
+      <c r="O13" s="7">
+        <v>5</v>
+      </c>
+      <c r="P13" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>3</v>
+      </c>
+      <c r="R13" s="7">
+        <v>3</v>
+      </c>
+      <c r="S13" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="8">
-        <v>4</v>
-      </c>
-      <c r="C14" s="8">
-        <v>1</v>
-      </c>
-      <c r="D14" s="8">
-        <v>1</v>
-      </c>
-      <c r="E14" s="8">
-        <v>4</v>
-      </c>
-      <c r="F14" s="8">
-        <v>2</v>
-      </c>
-      <c r="G14" s="8">
-        <v>3</v>
-      </c>
-      <c r="H14" s="8">
-        <v>4</v>
-      </c>
-      <c r="I14" s="8">
-        <v>5</v>
-      </c>
-      <c r="J14" s="8">
-        <v>3</v>
-      </c>
-      <c r="K14" s="8">
-        <v>3</v>
-      </c>
-      <c r="L14" s="8">
-        <v>4</v>
-      </c>
-      <c r="M14" s="8">
-        <v>5</v>
-      </c>
-      <c r="N14" s="8">
-        <v>5</v>
-      </c>
-      <c r="O14" s="8">
-        <v>5</v>
-      </c>
-      <c r="P14" s="8">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>1</v>
-      </c>
-      <c r="R14" s="8">
-        <v>1</v>
-      </c>
-      <c r="S14" s="8">
+      <c r="B14" s="7">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>4</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2</v>
+      </c>
+      <c r="G14" s="7">
+        <v>3</v>
+      </c>
+      <c r="H14" s="7">
+        <v>4</v>
+      </c>
+      <c r="I14" s="7">
+        <v>5</v>
+      </c>
+      <c r="J14" s="7">
+        <v>3</v>
+      </c>
+      <c r="K14" s="7">
+        <v>3</v>
+      </c>
+      <c r="L14" s="7">
+        <v>4</v>
+      </c>
+      <c r="M14" s="7">
+        <v>5</v>
+      </c>
+      <c r="N14" s="7">
+        <v>5</v>
+      </c>
+      <c r="O14" s="7">
+        <v>5</v>
+      </c>
+      <c r="P14" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>1</v>
+      </c>
+      <c r="R14" s="7">
+        <v>1</v>
+      </c>
+      <c r="S14" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="8">
-        <v>3</v>
-      </c>
-      <c r="C15" s="8">
-        <v>1</v>
-      </c>
-      <c r="D15" s="8">
-        <v>2</v>
-      </c>
-      <c r="E15" s="8">
-        <v>2</v>
-      </c>
-      <c r="F15" s="8">
-        <v>1</v>
-      </c>
-      <c r="G15" s="8">
-        <v>1</v>
-      </c>
-      <c r="H15" s="8">
-        <v>1</v>
-      </c>
-      <c r="I15" s="8">
-        <v>2</v>
-      </c>
-      <c r="J15" s="8">
-        <v>1</v>
-      </c>
-      <c r="K15" s="8">
-        <v>1</v>
-      </c>
-      <c r="L15" s="8">
-        <v>1</v>
-      </c>
-      <c r="M15" s="8">
-        <v>4</v>
-      </c>
-      <c r="N15" s="8">
-        <v>3</v>
-      </c>
-      <c r="O15" s="8">
-        <v>4</v>
-      </c>
-      <c r="P15" s="8">
-        <v>4</v>
-      </c>
-      <c r="Q15" s="8">
-        <v>2</v>
-      </c>
-      <c r="R15" s="8">
-        <v>2</v>
-      </c>
-      <c r="S15" s="8">
+      <c r="B15" s="7">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2</v>
+      </c>
+      <c r="E15" s="7">
+        <v>2</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7">
+        <v>1</v>
+      </c>
+      <c r="H15" s="7">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7">
+        <v>2</v>
+      </c>
+      <c r="J15" s="7">
+        <v>1</v>
+      </c>
+      <c r="K15" s="7">
+        <v>1</v>
+      </c>
+      <c r="L15" s="7">
+        <v>1</v>
+      </c>
+      <c r="M15" s="7">
+        <v>4</v>
+      </c>
+      <c r="N15" s="7">
+        <v>3</v>
+      </c>
+      <c r="O15" s="7">
+        <v>4</v>
+      </c>
+      <c r="P15" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>2</v>
+      </c>
+      <c r="R15" s="7">
+        <v>2</v>
+      </c>
+      <c r="S15" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="8">
-        <v>4</v>
-      </c>
-      <c r="C16" s="8">
-        <v>4</v>
-      </c>
-      <c r="D16" s="8">
-        <v>4</v>
-      </c>
-      <c r="E16" s="8">
-        <v>5</v>
-      </c>
-      <c r="F16" s="8">
-        <v>4</v>
-      </c>
-      <c r="G16" s="8">
-        <v>1</v>
-      </c>
-      <c r="H16" s="8">
-        <v>1</v>
-      </c>
-      <c r="I16" s="8">
-        <v>4</v>
-      </c>
-      <c r="J16" s="8">
-        <v>1</v>
-      </c>
-      <c r="K16" s="8">
-        <v>4</v>
-      </c>
-      <c r="L16" s="8">
-        <v>4</v>
-      </c>
-      <c r="M16" s="8">
-        <v>5</v>
-      </c>
-      <c r="N16" s="8">
-        <v>5</v>
-      </c>
-      <c r="O16" s="8">
-        <v>5</v>
-      </c>
-      <c r="P16" s="8">
-        <v>5</v>
-      </c>
-      <c r="Q16" s="8">
-        <v>1</v>
-      </c>
-      <c r="R16" s="8">
-        <v>5</v>
-      </c>
-      <c r="S16" s="8">
+      <c r="B16" s="7">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7">
+        <v>4</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4</v>
+      </c>
+      <c r="E16" s="7">
+        <v>5</v>
+      </c>
+      <c r="F16" s="7">
+        <v>4</v>
+      </c>
+      <c r="G16" s="7">
+        <v>1</v>
+      </c>
+      <c r="H16" s="7">
+        <v>1</v>
+      </c>
+      <c r="I16" s="7">
+        <v>4</v>
+      </c>
+      <c r="J16" s="7">
+        <v>1</v>
+      </c>
+      <c r="K16" s="7">
+        <v>4</v>
+      </c>
+      <c r="L16" s="7">
+        <v>4</v>
+      </c>
+      <c r="M16" s="7">
+        <v>5</v>
+      </c>
+      <c r="N16" s="7">
+        <v>5</v>
+      </c>
+      <c r="O16" s="7">
+        <v>5</v>
+      </c>
+      <c r="P16" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>1</v>
+      </c>
+      <c r="R16" s="7">
+        <v>5</v>
+      </c>
+      <c r="S16" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="8">
-        <v>3</v>
-      </c>
-      <c r="C17" s="8">
-        <v>3</v>
-      </c>
-      <c r="D17" s="8">
-        <v>3</v>
-      </c>
-      <c r="E17" s="8">
-        <v>4</v>
-      </c>
-      <c r="F17" s="8">
-        <v>3</v>
-      </c>
-      <c r="G17" s="8">
-        <v>4</v>
-      </c>
-      <c r="H17" s="8">
-        <v>1</v>
-      </c>
-      <c r="I17" s="8">
-        <v>1</v>
-      </c>
-      <c r="J17" s="8">
-        <v>1</v>
-      </c>
-      <c r="K17" s="8">
-        <v>1</v>
-      </c>
-      <c r="L17" s="8">
-        <v>1</v>
-      </c>
-      <c r="M17" s="8">
-        <v>5</v>
-      </c>
-      <c r="N17" s="8">
-        <v>5</v>
-      </c>
-      <c r="O17" s="8">
-        <v>4</v>
-      </c>
-      <c r="P17" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q17" s="8">
-        <v>1</v>
-      </c>
-      <c r="R17" s="8">
-        <v>1</v>
-      </c>
-      <c r="S17" s="8">
+      <c r="A17" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="7">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7">
+        <v>3</v>
+      </c>
+      <c r="D17" s="7">
+        <v>3</v>
+      </c>
+      <c r="E17" s="7">
+        <v>4</v>
+      </c>
+      <c r="F17" s="7">
+        <v>3</v>
+      </c>
+      <c r="G17" s="7">
+        <v>4</v>
+      </c>
+      <c r="H17" s="7">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7">
+        <v>1</v>
+      </c>
+      <c r="J17" s="7">
+        <v>1</v>
+      </c>
+      <c r="K17" s="7">
+        <v>1</v>
+      </c>
+      <c r="L17" s="7">
+        <v>1</v>
+      </c>
+      <c r="M17" s="7">
+        <v>5</v>
+      </c>
+      <c r="N17" s="7">
+        <v>5</v>
+      </c>
+      <c r="O17" s="7">
+        <v>4</v>
+      </c>
+      <c r="P17" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>1</v>
+      </c>
+      <c r="R17" s="7">
+        <v>1</v>
+      </c>
+      <c r="S17" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="8">
-        <v>5</v>
-      </c>
-      <c r="C18" s="8">
-        <v>3</v>
-      </c>
-      <c r="D18" s="8">
-        <v>2</v>
-      </c>
-      <c r="E18" s="8">
-        <v>3</v>
-      </c>
-      <c r="F18" s="8">
-        <v>2</v>
-      </c>
-      <c r="G18" s="8">
-        <v>2</v>
-      </c>
-      <c r="H18" s="8">
-        <v>2</v>
-      </c>
-      <c r="I18" s="8">
-        <v>2</v>
-      </c>
-      <c r="J18" s="8">
-        <v>2</v>
-      </c>
-      <c r="K18" s="8">
-        <v>2</v>
-      </c>
-      <c r="L18" s="8">
-        <v>2</v>
-      </c>
-      <c r="M18" s="8">
-        <v>3</v>
-      </c>
-      <c r="N18" s="8">
-        <v>3</v>
-      </c>
-      <c r="O18" s="8">
-        <v>3</v>
-      </c>
-      <c r="P18" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="8">
-        <v>4</v>
-      </c>
-      <c r="R18" s="8">
-        <v>5</v>
-      </c>
-      <c r="S18" s="8">
+      <c r="B18" s="7">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7">
+        <v>3</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7">
+        <v>3</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2</v>
+      </c>
+      <c r="G18" s="7">
+        <v>2</v>
+      </c>
+      <c r="H18" s="7">
+        <v>2</v>
+      </c>
+      <c r="I18" s="7">
+        <v>2</v>
+      </c>
+      <c r="J18" s="7">
+        <v>2</v>
+      </c>
+      <c r="K18" s="7">
+        <v>2</v>
+      </c>
+      <c r="L18" s="7">
+        <v>2</v>
+      </c>
+      <c r="M18" s="7">
+        <v>3</v>
+      </c>
+      <c r="N18" s="7">
+        <v>3</v>
+      </c>
+      <c r="O18" s="7">
+        <v>3</v>
+      </c>
+      <c r="P18" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>4</v>
+      </c>
+      <c r="R18" s="7">
+        <v>5</v>
+      </c>
+      <c r="S18" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="8">
-        <v>3</v>
-      </c>
-      <c r="C19" s="8">
-        <v>1</v>
-      </c>
-      <c r="D19" s="8">
-        <v>2</v>
-      </c>
-      <c r="E19" s="8">
-        <v>3</v>
-      </c>
-      <c r="F19" s="8">
-        <v>2</v>
-      </c>
-      <c r="G19" s="8">
-        <v>2</v>
-      </c>
-      <c r="H19" s="8">
-        <v>2</v>
-      </c>
-      <c r="I19" s="8">
-        <v>3</v>
-      </c>
-      <c r="J19" s="8">
-        <v>1</v>
-      </c>
-      <c r="K19" s="8">
-        <v>1</v>
-      </c>
-      <c r="L19" s="8">
-        <v>1</v>
-      </c>
-      <c r="M19" s="8">
-        <v>5</v>
-      </c>
-      <c r="N19" s="8">
-        <v>3</v>
-      </c>
-      <c r="O19" s="8">
-        <v>4</v>
-      </c>
-      <c r="P19" s="8">
-        <v>3</v>
-      </c>
-      <c r="Q19" s="8">
-        <v>4</v>
-      </c>
-      <c r="R19" s="8">
-        <v>4</v>
-      </c>
-      <c r="S19" s="8">
+      <c r="A19" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="7">
+        <v>3</v>
+      </c>
+      <c r="C19" s="7">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
+        <v>2</v>
+      </c>
+      <c r="E19" s="7">
+        <v>3</v>
+      </c>
+      <c r="F19" s="7">
+        <v>2</v>
+      </c>
+      <c r="G19" s="7">
+        <v>2</v>
+      </c>
+      <c r="H19" s="7">
+        <v>2</v>
+      </c>
+      <c r="I19" s="7">
+        <v>3</v>
+      </c>
+      <c r="J19" s="7">
+        <v>1</v>
+      </c>
+      <c r="K19" s="7">
+        <v>1</v>
+      </c>
+      <c r="L19" s="7">
+        <v>1</v>
+      </c>
+      <c r="M19" s="7">
+        <v>5</v>
+      </c>
+      <c r="N19" s="7">
+        <v>3</v>
+      </c>
+      <c r="O19" s="7">
+        <v>4</v>
+      </c>
+      <c r="P19" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>4</v>
+      </c>
+      <c r="R19" s="7">
+        <v>4</v>
+      </c>
+      <c r="S19" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="8">
-        <v>5</v>
-      </c>
-      <c r="C20" s="8">
-        <v>4</v>
-      </c>
-      <c r="D20" s="8">
-        <v>3</v>
-      </c>
-      <c r="E20" s="8">
-        <v>3</v>
-      </c>
-      <c r="F20" s="8">
-        <v>3</v>
-      </c>
-      <c r="G20" s="8">
-        <v>3</v>
-      </c>
-      <c r="H20" s="8">
-        <v>5</v>
-      </c>
-      <c r="I20" s="8">
-        <v>5</v>
-      </c>
-      <c r="J20" s="8">
-        <v>3</v>
-      </c>
-      <c r="K20" s="8">
-        <v>3</v>
-      </c>
-      <c r="L20" s="8">
-        <v>3</v>
-      </c>
-      <c r="M20" s="8">
-        <v>5</v>
-      </c>
-      <c r="N20" s="8">
-        <v>4</v>
-      </c>
-      <c r="O20" s="8">
-        <v>5</v>
-      </c>
-      <c r="P20" s="8">
-        <v>5</v>
-      </c>
-      <c r="Q20" s="8">
-        <v>3</v>
-      </c>
-      <c r="R20" s="8">
-        <v>3</v>
-      </c>
-      <c r="S20" s="8">
+      <c r="A20" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="7">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7">
+        <v>4</v>
+      </c>
+      <c r="D20" s="7">
+        <v>3</v>
+      </c>
+      <c r="E20" s="7">
+        <v>3</v>
+      </c>
+      <c r="F20" s="7">
+        <v>3</v>
+      </c>
+      <c r="G20" s="7">
+        <v>3</v>
+      </c>
+      <c r="H20" s="7">
+        <v>5</v>
+      </c>
+      <c r="I20" s="7">
+        <v>5</v>
+      </c>
+      <c r="J20" s="7">
+        <v>3</v>
+      </c>
+      <c r="K20" s="7">
+        <v>3</v>
+      </c>
+      <c r="L20" s="7">
+        <v>3</v>
+      </c>
+      <c r="M20" s="7">
+        <v>5</v>
+      </c>
+      <c r="N20" s="7">
+        <v>4</v>
+      </c>
+      <c r="O20" s="7">
+        <v>5</v>
+      </c>
+      <c r="P20" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>3</v>
+      </c>
+      <c r="R20" s="7">
+        <v>3</v>
+      </c>
+      <c r="S20" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2097,7 +2335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2106,7 +2344,7 @@
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="10" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="1.6640625" customWidth="1"/>
@@ -2114,34 +2352,34 @@
     <col min="9" max="9" width="42.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="3" cm="1">
@@ -2153,7 +2391,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A2,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>610</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
         <f t="shared" ref="D2:D19" si="0">IF(C2&gt;0,B2/C2,0)</f>
         <v>0.49508196721311476</v>
       </c>
@@ -2165,7 +2403,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A2,CHAR(160)," ")))),"")</f>
         <v>3</v>
       </c>
-      <c r="H2" s="6" t="str" cm="1">
+      <c r="H2" s="5" t="str" cm="1">
         <f t="array" ref="H2">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2176,7 +2414,7 @@
 "")</f>
         <v>Customer Service &amp; Sales, Schedule Flexibility, Social Personality</v>
       </c>
-      <c r="I2" s="6" t="str" cm="1">
+      <c r="I2" s="5" t="str" cm="1">
         <f t="array" ref="I2">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2188,8 +2426,8 @@
         <v>Proximity to Customers, Product Diversity, Floral Design</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="3" cm="1">
@@ -2201,7 +2439,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A3,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>550</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
@@ -2213,7 +2451,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A3,CHAR(160)," ")))),"")</f>
         <v>2</v>
       </c>
-      <c r="H3" s="6" t="str" cm="1">
+      <c r="H3" s="5" t="str" cm="1">
         <f t="array" ref="H3">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2224,7 +2462,7 @@
 "")</f>
         <v>Customer Service &amp; Sales, Personal Connections</v>
       </c>
-      <c r="I3" s="6" t="str" cm="1">
+      <c r="I3" s="5" t="str" cm="1">
         <f t="array" ref="I3">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2237,7 +2475,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="3" cm="1">
@@ -2249,7 +2487,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A4,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>560</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <f t="shared" si="0"/>
         <v>0.52142857142857146</v>
       </c>
@@ -2261,7 +2499,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A4,CHAR(160)," ")))),"")</f>
         <v>1</v>
       </c>
-      <c r="H4" s="6" t="str" cm="1">
+      <c r="H4" s="5" t="str" cm="1">
         <f t="array" ref="H4">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2272,7 +2510,7 @@
 "")</f>
         <v>Personal Connections</v>
       </c>
-      <c r="I4" s="6" t="str" cm="1">
+      <c r="I4" s="5" t="str" cm="1">
         <f t="array" ref="I4">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2284,8 +2522,8 @@
         <v>Proximity to Customers, Product Diversity, Floral Design</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="3" cm="1">
@@ -2297,7 +2535,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A5,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>590</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <f t="shared" si="0"/>
         <v>0.50169491525423726</v>
       </c>
@@ -2309,7 +2547,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A5,CHAR(160)," ")))),"")</f>
         <v>2</v>
       </c>
-      <c r="H5" s="6" t="str" cm="1">
+      <c r="H5" s="5" t="str" cm="1">
         <f t="array" ref="H5">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2320,7 +2558,7 @@
 "")</f>
         <v>Customer Service &amp; Sales, Schedule Flexibility</v>
       </c>
-      <c r="I5" s="6" t="str" cm="1">
+      <c r="I5" s="5" t="str" cm="1">
         <f t="array" ref="I5">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2329,11 +2567,11 @@
       )
    ),
 "")</f>
-        <v>Proximity to Customers, Product Diversity, Floral Design, Color Comprehension and Accuracy</v>
+        <v>Proximity to Customers, Product Diversity, Floral Design, Color Comprehension &amp; Accuracy</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="3" cm="1">
@@ -2345,7 +2583,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A6,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>490</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <f t="shared" si="0"/>
         <v>0.50408163265306127</v>
       </c>
@@ -2357,7 +2595,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A6,CHAR(160)," ")))),"")</f>
         <v>0</v>
       </c>
-      <c r="H6" s="6" t="str" cm="1">
+      <c r="H6" s="5" t="str" cm="1">
         <f t="array" ref="H6">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2368,7 +2606,7 @@
 "")</f>
         <v/>
       </c>
-      <c r="I6" s="6" t="str" cm="1">
+      <c r="I6" s="5" t="str" cm="1">
         <f t="array" ref="I6">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2381,7 +2619,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="3" cm="1">
@@ -2393,7 +2631,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A7,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>390</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <f t="shared" si="0"/>
         <v>0.49487179487179489</v>
       </c>
@@ -2405,7 +2643,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A7,CHAR(160)," ")))),"")</f>
         <v>0</v>
       </c>
-      <c r="H7" s="6" t="str" cm="1">
+      <c r="H7" s="5" t="str" cm="1">
         <f t="array" ref="H7">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2416,7 +2654,7 @@
 "")</f>
         <v/>
       </c>
-      <c r="I7" s="6" t="str" cm="1">
+      <c r="I7" s="5" t="str" cm="1">
         <f t="array" ref="I7">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2425,11 +2663,11 @@
       )
    ),
 "")</f>
-        <v>Color Comprehension and Accuracy</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+        <v>Color Comprehension &amp; Accuracy</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="3" cm="1">
@@ -2441,19 +2679,19 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A8,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>430</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <f t="shared" si="0"/>
         <v>0.4697674418604651</v>
       </c>
-      <c r="E8" s="15" t="str">
+      <c r="E8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Stretch</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="3">
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A8,CHAR(160)," ")))),"")</f>
         <v>1</v>
       </c>
-      <c r="H8" s="6" t="str" cm="1">
+      <c r="H8" s="5" t="str" cm="1">
         <f t="array" ref="H8">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2464,7 +2702,7 @@
 "")</f>
         <v>Schedule Flexibility</v>
       </c>
-      <c r="I8" s="6" t="str" cm="1">
+      <c r="I8" s="5" t="str" cm="1">
         <f t="array" ref="I8">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2476,8 +2714,8 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="3" cm="1">
@@ -2489,19 +2727,19 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A9,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>520</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <f t="shared" si="0"/>
         <v>0.50384615384615383</v>
       </c>
-      <c r="E9" s="15" t="str">
+      <c r="E9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Could Work</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="3">
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A9,CHAR(160)," ")))),"")</f>
         <v>1</v>
       </c>
-      <c r="H9" s="6" t="str" cm="1">
+      <c r="H9" s="5" t="str" cm="1">
         <f t="array" ref="H9">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2512,7 +2750,7 @@
 "")</f>
         <v>Schedule Flexibility</v>
       </c>
-      <c r="I9" s="6" t="str" cm="1">
+      <c r="I9" s="5" t="str" cm="1">
         <f t="array" ref="I9">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2525,7 +2763,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="3" cm="1">
@@ -2537,7 +2775,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A10,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>360</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f t="shared" si="0"/>
         <v>0.46666666666666667</v>
       </c>
@@ -2549,7 +2787,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A10,CHAR(160)," ")))),"")</f>
         <v>0</v>
       </c>
-      <c r="H10" s="6" t="str" cm="1">
+      <c r="H10" s="5" t="str" cm="1">
         <f t="array" ref="H10">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2560,7 +2798,7 @@
 "")</f>
         <v/>
       </c>
-      <c r="I10" s="6" t="str" cm="1">
+      <c r="I10" s="5" t="str" cm="1">
         <f t="array" ref="I10">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2573,7 +2811,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="3" cm="1">
@@ -2585,7 +2823,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A11,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>430</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
         <v>0.50930232558139532</v>
       </c>
@@ -2597,7 +2835,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A11,CHAR(160)," ")))),"")</f>
         <v>1</v>
       </c>
-      <c r="H11" s="6" t="str" cm="1">
+      <c r="H11" s="5" t="str" cm="1">
         <f t="array" ref="H11">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2608,7 +2846,7 @@
 "")</f>
         <v>Professional Network</v>
       </c>
-      <c r="I11" s="6" t="str" cm="1">
+      <c r="I11" s="5" t="str" cm="1">
         <f t="array" ref="I11">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2620,8 +2858,8 @@
         <v>Proximity to Customers, Product Diversity, Floral Design</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="3" cm="1">
@@ -2633,7 +2871,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A12,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>430</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <f t="shared" si="0"/>
         <v>0.50697674418604655</v>
       </c>
@@ -2645,7 +2883,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A12,CHAR(160)," ")))),"")</f>
         <v>2</v>
       </c>
-      <c r="H12" s="6" t="str" cm="1">
+      <c r="H12" s="5" t="str" cm="1">
         <f t="array" ref="H12">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2656,7 +2894,7 @@
 "")</f>
         <v>Professional Network, Schedule Flexibility</v>
       </c>
-      <c r="I12" s="6" t="str" cm="1">
+      <c r="I12" s="5" t="str" cm="1">
         <f t="array" ref="I12">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2668,8 +2906,8 @@
         <v>Proximity to Customers, Product Diversity, Floral Design</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="3" cm="1">
@@ -2681,7 +2919,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A13,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>700</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="12">
         <f t="shared" si="0"/>
         <v>0.49428571428571427</v>
       </c>
@@ -2693,7 +2931,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A13,CHAR(160)," ")))),"")</f>
         <v>3</v>
       </c>
-      <c r="H13" s="6" t="str" cm="1">
+      <c r="H13" s="5" t="str" cm="1">
         <f t="array" ref="H13">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2702,9 +2940,9 @@
       )
    ),
 "")</f>
-        <v>Customer Service &amp; Sales, Schedule Flexibility, Stress and Risk Tolerance</v>
-      </c>
-      <c r="I13" s="6" t="str" cm="1">
+        <v>Customer Service &amp; Sales, Schedule Flexibility, Stress &amp; Risk Tolerance</v>
+      </c>
+      <c r="I13" s="5" t="str" cm="1">
         <f t="array" ref="I13">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2713,11 +2951,11 @@
       )
    ),
 "")</f>
-        <v>Product Diversity, Floral Design, Color Comprehension and Accuracy</v>
+        <v>Product Diversity, Floral Design, Color Comprehension &amp; Accuracy</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="3" cm="1">
@@ -2729,19 +2967,19 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A14,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>640</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="12">
         <f t="shared" si="0"/>
         <v>0.50937500000000002</v>
       </c>
-      <c r="E14" s="15" t="str">
+      <c r="E14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Could Work</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="3">
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A14,CHAR(160)," ")))),"")</f>
         <v>1</v>
       </c>
-      <c r="H14" s="6" t="str" cm="1">
+      <c r="H14" s="5" t="str" cm="1">
         <f t="array" ref="H14">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2752,7 +2990,7 @@
 "")</f>
         <v>Schedule Flexibility</v>
       </c>
-      <c r="I14" s="6" t="str" cm="1">
+      <c r="I14" s="5" t="str" cm="1">
         <f t="array" ref="I14">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2761,11 +2999,11 @@
       )
    ),
 "")</f>
-        <v>Product Diversity, Floral Design, Color Comprehension and Accuracy</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" ht="128" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+        <v>Product Diversity, Floral Design, Color Comprehension &amp; Accuracy</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="3" cm="1">
@@ -2777,7 +3015,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A15,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>660</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="12">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
@@ -2789,7 +3027,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A15,CHAR(160)," ")))),"")</f>
         <v>4</v>
       </c>
-      <c r="H15" s="6" t="str" cm="1">
+      <c r="H15" s="5" t="str" cm="1">
         <f t="array" ref="H15">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2798,9 +3036,9 @@
       )
    ),
 "")</f>
-        <v>Customer Service &amp; Sales, Professional Network, Schedule Flexibility, Stress and Risk Tolerance</v>
-      </c>
-      <c r="I15" s="6" t="str" cm="1">
+        <v>Customer Service &amp; Sales, Professional Network, Schedule Flexibility, Stress &amp; Risk Tolerance</v>
+      </c>
+      <c r="I15" s="5" t="str" cm="1">
         <f t="array" ref="I15">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2809,11 +3047,11 @@
       )
    ),
 "")</f>
-        <v>Product Diversity, Floral Design, Color Comprehension and Accuracy</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+        <v>Product Diversity, Floral Design, Color Comprehension &amp; Accuracy</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="3" cm="1">
@@ -2825,7 +3063,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A16,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>590</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="12">
         <f t="shared" si="0"/>
         <v>0.51186440677966105</v>
       </c>
@@ -2837,7 +3075,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A16,CHAR(160)," ")))),"")</f>
         <v>2</v>
       </c>
-      <c r="H16" s="6" t="str" cm="1">
+      <c r="H16" s="5" t="str" cm="1">
         <f t="array" ref="H16">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2848,7 +3086,7 @@
 "")</f>
         <v>Professional Network, Schedule Flexibility</v>
       </c>
-      <c r="I16" s="6" t="str" cm="1">
+      <c r="I16" s="5" t="str" cm="1">
         <f t="array" ref="I16">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2860,8 +3098,8 @@
         <v>Proximity to Customers, Product Diversity, Floral Design</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" ht="112" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B17" s="3" cm="1">
@@ -2873,7 +3111,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A17,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>590</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="12">
         <f t="shared" si="0"/>
         <v>0.43728813559322033</v>
       </c>
@@ -2885,7 +3123,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A17,CHAR(160)," ")))),"")</f>
         <v>4</v>
       </c>
-      <c r="H17" s="6" t="str" cm="1">
+      <c r="H17" s="5" t="str" cm="1">
         <f t="array" ref="H17">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2894,9 +3132,9 @@
       )
    ),
 "")</f>
-        <v>Customer Service &amp; Sales, Customer-Friendly Amenities, Social Personality, Stress and Risk Tolerance</v>
-      </c>
-      <c r="I17" s="6" t="str" cm="1">
+        <v>Customer Service &amp; Sales, Customer-Friendly Amenities, Social Personality, Stress &amp; Risk Tolerance</v>
+      </c>
+      <c r="I17" s="5" t="str" cm="1">
         <f t="array" ref="I17">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2908,8 +3146,8 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" ht="112" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:9" s="3" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="3" cm="1">
@@ -2921,7 +3159,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A18,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>650</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="12">
         <f t="shared" si="0"/>
         <v>0.47076923076923077</v>
       </c>
@@ -2933,7 +3171,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A18,CHAR(160)," ")))),"")</f>
         <v>4</v>
       </c>
-      <c r="H18" s="6" t="str" cm="1">
+      <c r="H18" s="5" t="str" cm="1">
         <f t="array" ref="H18">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2942,9 +3180,9 @@
       )
    ),
 "")</f>
-        <v>Customer Service &amp; Sales, Customer-Friendly Amenities, Social Personality, Stress and Risk Tolerance</v>
-      </c>
-      <c r="I18" s="6" t="str" cm="1">
+        <v>Customer Service &amp; Sales, Customer-Friendly Amenities, Social Personality, Stress &amp; Risk Tolerance</v>
+      </c>
+      <c r="I18" s="5" t="str" cm="1">
         <f t="array" ref="I18">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2956,8 +3194,8 @@
         <v>Product Diversity, Floral Design</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+    <row r="19" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="3" cm="1">
@@ -2969,7 +3207,7 @@
         <f>IFERROR(10*SUM(INDEX(Weights!$B$2:$ZZ$20,0,MATCH($A19,Weights!$B$1:$ZZ$1,0))),0)</f>
         <v>470</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="12">
         <f t="shared" si="0"/>
         <v>0.46382978723404256</v>
       </c>
@@ -2981,7 +3219,7 @@
         <f>IFERROR(SUMPRODUCT((--Inputs!$B$2:$B$20&lt;=3)*(--(Weights!$B$2:$S$20)&gt;=4)*(TRIM(SUBSTITUTE(Weights!$B$1:$S$1,CHAR(160)," "))=TRIM(SUBSTITUTE($A19,CHAR(160)," ")))),"")</f>
         <v>2</v>
       </c>
-      <c r="H19" s="6" t="str" cm="1">
+      <c r="H19" s="5" t="str" cm="1">
         <f t="array" ref="H19">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -2990,9 +3228,9 @@
       )
    ),
 "")</f>
-        <v>Customer-Friendly Amenities, Stress and Risk Tolerance</v>
-      </c>
-      <c r="I19" s="6" t="str" cm="1">
+        <v>Customer-Friendly Amenities, Stress &amp; Risk Tolerance</v>
+      </c>
+      <c r="I19" s="5" t="str" cm="1">
         <f t="array" ref="I19">IFERROR(
    _xlfn.TEXTJOIN(", ",TRUE,
       _xlfn._xlws.FILTER(Weights!$A$2:$A$20,
@@ -3010,6 +3248,511 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843472F9-263E-924A-9F9A-DC61CDC4480E}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="85.1640625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4685398-D085-6B47-BDBF-4D7FCE78162F}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="16" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -3183,7 +3926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added code for testing creation of Top 3 narratives for testing in Streamlit. These will eventually go inside a Flodesk email but for now they will be easy to visualize via Streamlit.
</commit_message>
<xml_diff>
--- a/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
+++ b/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Downloads/rsc-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D00F2D-483C-5848-8D15-C09C7E6F2EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A678C478-A25F-464F-BF52-56F33C8D6E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="270">
   <si>
     <t>Section</t>
   </si>
@@ -820,6 +820,63 @@
   </si>
   <si>
     <t>Without marketing, potential customers may not even know bulk buckets are an option, limiting sales.</t>
+  </si>
+  <si>
+    <t>Strong marketing helps you reach customers, even those who hadn't realized that DIY flowers might be a great option for their event.</t>
+  </si>
+  <si>
+    <t>Customers buying buckets want value and flexibility; diversity in ingredients makes the purchase worthwhile.</t>
+  </si>
+  <si>
+    <t>A diverse crop plan ensures your bulk buckets feel plentiful and include the mix of floral ingredients customers trying to create their own designs will need.</t>
+  </si>
+  <si>
+    <t>Without enough diversity of floral ingredients, customers may be frustrated by the difficulty in pulling together balanced, attractive designs.</t>
+  </si>
+  <si>
+    <t>Strong planning and succession planting keep stems available in the quantities promised, so customers get what they expect when they placed their order.</t>
+  </si>
+  <si>
+    <t>Without reliable production, you may fall short on promised quantities, leading to unhappy customers and last-minute scrambles.</t>
+  </si>
+  <si>
+    <t>Bulk orders are often tied to specific events; predictability is essential for delivering promised volume on time.</t>
+  </si>
+  <si>
+    <t>Bulk buckets still depend on thoughtful curation; customers need the right balance of ingredients to succeed in DIY design.</t>
+  </si>
+  <si>
+    <t>Without design sense, buckets may be lopsided or impractical, frustrating customers who expect them to translate easily into designs.</t>
+  </si>
+  <si>
+    <t>Even though customers are arranging themselves, a good design eye helps you assemble balanced buckets with usable ratios of different floral ingredients.</t>
+  </si>
+  <si>
+    <t>Florists depend on consistent quality and timing; your infrastructure is what protects stems from harvest to handoff.</t>
+  </si>
+  <si>
+    <t>Without solid infrastructure, flowers may arrive wilted, damaged, or late, undermining trust with florists.</t>
+  </si>
+  <si>
+    <t>Strong infrastructure — from coolers to delivery systems — keeps stems fresh and organized, ensuring florists receive high-quality product.</t>
+  </si>
+  <si>
+    <t>Florists build their orders and commitments around availability; they need dependable quantities and timing.</t>
+  </si>
+  <si>
+    <t>Without predictability, florists can’t plan their own designs or events, and they may turn to other suppliers.</t>
+  </si>
+  <si>
+    <t>Reliable production and succession planting give florists confidence they can count on you week after week.</t>
+  </si>
+  <si>
+    <t>Without attention to color requests, you risk producing flowers that don’t align with florist expectations, which affect repeat sales and weaken trust.</t>
+  </si>
+  <si>
+    <t>Florists often design with color first; being able to understand their needs and communicate subleties in coloration is often critical to their success.</t>
+  </si>
+  <si>
+    <t>Strong color awareness ensures you grow and supply palettes that match florist demand; making you their go-to source for locally grown flowers.</t>
   </si>
 </sst>
 </file>
@@ -4409,8 +4466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EBBEDC-5414-B442-BDB4-EC1529FD0ACE}">
   <dimension ref="A1:G343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5820,6 +5877,9 @@
       <c r="D79" s="14">
         <v>5</v>
       </c>
+      <c r="E79" s="5" t="s">
+        <v>251</v>
+      </c>
       <c r="F79" s="5" t="s">
         <v>250</v>
       </c>
@@ -5841,7 +5901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>133</v>
       </c>
@@ -5855,7 +5915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>133</v>
       </c>
@@ -5869,7 +5929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>133</v>
       </c>
@@ -5883,7 +5943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>133</v>
       </c>
@@ -5897,7 +5957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>133</v>
       </c>
@@ -5911,7 +5971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>133</v>
       </c>
@@ -5924,8 +5984,17 @@
       <c r="D86" s="14">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>133</v>
       </c>
@@ -5939,7 +6008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>133</v>
       </c>
@@ -5953,7 +6022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>133</v>
       </c>
@@ -5966,8 +6035,17 @@
       <c r="D89" s="14">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>133</v>
       </c>
@@ -5981,7 +6059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>133</v>
       </c>
@@ -5995,7 +6073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>133</v>
       </c>
@@ -6008,8 +6086,17 @@
       <c r="D92" s="14">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>133</v>
       </c>
@@ -6023,7 +6110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>133</v>
       </c>
@@ -6037,7 +6124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>133</v>
       </c>
@@ -6051,7 +6138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>133</v>
       </c>
@@ -6065,7 +6152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>134</v>
       </c>
@@ -6079,7 +6166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>134</v>
       </c>
@@ -6093,7 +6180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>134</v>
       </c>
@@ -6107,7 +6194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>134</v>
       </c>
@@ -6121,7 +6208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>134</v>
       </c>
@@ -6135,7 +6222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>134</v>
       </c>
@@ -6149,7 +6236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>134</v>
       </c>
@@ -6163,7 +6250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>134</v>
       </c>
@@ -6177,7 +6264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>134</v>
       </c>
@@ -6191,7 +6278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>134</v>
       </c>
@@ -6205,7 +6292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>134</v>
       </c>
@@ -6218,8 +6305,17 @@
       <c r="D107" s="14">
         <v>4</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>134</v>
       </c>
@@ -6232,8 +6328,17 @@
       <c r="D108" s="14">
         <v>4</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>134</v>
       </c>
@@ -6247,7 +6352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>134</v>
       </c>
@@ -6261,7 +6366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>134</v>
       </c>
@@ -6275,7 +6380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>134</v>
       </c>
@@ -6287,6 +6392,15 @@
       </c>
       <c r="D112" s="14">
         <v>4</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added code that builds narratives text in Excel file, using math/logic aimed at finding the needle movers (two highest and one lowest weighted scores)
</commit_message>
<xml_diff>
--- a/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
+++ b/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Downloads/rsc-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A678C478-A25F-464F-BF52-56F33C8D6E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB4E07A-0D20-6D4F-A435-475FA4986C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -537,105 +537,6 @@
     <t>Interactive Events</t>
   </si>
   <si>
-    <t>Your strong customer service skills mean you’ll thrive at markets, where friendly interaction and repeat relationships are what keep customers coming back week after week.</t>
-  </si>
-  <si>
-    <t>Farmers Markets are built on direct interactions — chatting with shoppers, building loyalty, and standing out from the crowd. Success depends heavily on your ability to connect and sell face-to-face.</t>
-  </si>
-  <si>
-    <t>Without strong sales and people skills, it’s easy to get overlooked in a busy market. Customers may gravitate toward vendors who are more engaging or approachable.</t>
-  </si>
-  <si>
-    <t>Being close to your market makes it easier to transport flowers, keep them fresh, and build a loyal base of repeat customers.</t>
-  </si>
-  <si>
-    <t>If you’re far from a good market, long drives and time on the road eat into profits and cut into time on the farm.</t>
-  </si>
-  <si>
-    <t>Markets require weekly participation and fresh product; proximity to a strong customer base is a key driver of profitability and efficiency.</t>
-  </si>
-  <si>
-    <t>Without enough variety, it’s hard to build mixed bouquets, which farmers market customers tend to place a high value on.</t>
-  </si>
-  <si>
-    <t>Having a wide range of flowers means you can create the abundant mixed bouquets that customers expect at market, and your stand will look full and appealing.</t>
-  </si>
-  <si>
-    <t>Mixed bouquets are almost a requirement at farmers markets, and doing them well depends on having diverse ingredients to work with.</t>
-  </si>
-  <si>
-    <t>A lack of infrastructure makes your life a lot harder and--worst case--leads to wilted flowers, chaotic setup, and unnecessary stress before customers even arrive.</t>
-  </si>
-  <si>
-    <t>With solid infrastructure like coolers, tents, and ways to transport flowers safely, you’ll arrive prepared and be able to offer the freshest possible flowers.</t>
-  </si>
-  <si>
-    <t>The logistics of transporting, storing, and displaying flowers weekly are demanding; without infrastructure, quality and presentation suffer.</t>
-  </si>
-  <si>
-    <t>A consistent presence at market is critical to building loyal customers. When shoppers know you’ll be there every week with abundant flowers, they’ll seek out your booth instead of buying from the first vendor they see.</t>
-  </si>
-  <si>
-    <t>Careful crop planning and succession planting keep harvests steady, ensuring you have abundant stems every week to fill buckets and build market bouquets.</t>
-  </si>
-  <si>
-    <t>Without strong planning and successions, harvests may come in flushes, leaving you short on product some weeks and unable to meet customer demand.</t>
-  </si>
-  <si>
-    <t>If the market’s schedule conflicts with immovable commitments (like kids’ activities), showing up consistently will be difficult or impossible.</t>
-  </si>
-  <si>
-    <t>Having flexibility in your schedule that matches the market’s rhythm — including harvest, bouquet prep, and the market itself — makes it easier to commit week after week.</t>
-  </si>
-  <si>
-    <t>Farmers markets run on fixed days and times, and success depends on aligning your farm work and personal life to that schedule.</t>
-  </si>
-  <si>
-    <t>Mixed bouquets are the core market product at farmers markets; design skill is directly tied to your ability to attract customers to your booth and keep them coming back.</t>
-  </si>
-  <si>
-    <t>Without solid design skills, your mixed bouquets may look awkward or less professional, making it harder to compete with other vendors.</t>
-  </si>
-  <si>
-    <t>Strong design skills help you build mixed bouquets that are beautiful, balanced, and irresistible on the market table.</t>
-  </si>
-  <si>
-    <t>An outgoing, approachable personality helps you connect with customers, build loyalty, and create a welcoming booth atmosphere.</t>
-  </si>
-  <si>
-    <t>If social interaction drains you, markets may feel exhausting and hinder your ability to engage with buyers.</t>
-  </si>
-  <si>
-    <t>Markets are social by nature — success often depends as much on your presence and demeanor as on the flowers themselves.</t>
-  </si>
-  <si>
-    <t>trong organization and time management let you juggle harvesting, bouquet-making, and market prep without burning out — and ensure you arrive on time, fully prepared, and set up before the crowds arrive.</t>
-  </si>
-  <si>
-    <t>Poor organization can make market days chaotic — forgotten supplies, rushed prep, or late arrival. At many markets, arriving late can even mean losing your spot or being barred from setting up.</t>
-  </si>
-  <si>
-    <t>Farmers markets place firm demands on punctuality and preparedness. With immovable weekly deadlines, only growers with solid time management can consistently show up ready and on time.</t>
-  </si>
-  <si>
-    <t>Unlike a farmers market, subscriptions require you to drive sign-ups yourself. Marketing is essential for attracting customers.</t>
-  </si>
-  <si>
-    <t>Good marketing skills can help you attract new subscribers, highlight the value of your bouquets, and keep your subscriber list full.</t>
-  </si>
-  <si>
-    <t>Without strong marketing capabilities, your subscriber list may stay small or fail to grow.</t>
-  </si>
-  <si>
-    <t>Leveraging personal networks makes it easier to find your first subscribers, as friends, colleagues, and local contacts are often the earliest supporters.</t>
-  </si>
-  <si>
-    <t>Without strong personal connections, launching a subscription can be slow, as it’s harder to build momentum and trust at the start.</t>
-  </si>
-  <si>
-    <t>Many subscription programs start small and grow by word of mouth. A farmer’s existing relationships often determine how quickly a subscriber list fills.</t>
-  </si>
-  <si>
     <t>Subscriptions depend on regular, reliable fulfillment; proximity to customer helps keep delivery costs manageable.</t>
   </si>
   <si>
@@ -645,51 +546,6 @@
     <t>If customers are spread out, long drives can add costs, stress, and even the risk of wilted flowers.</t>
   </si>
   <si>
-    <t>Subscriptions are a promise; predictability underpins the entire model, reducing the likelihood that you have to cancel or reschedule your promised product.</t>
-  </si>
-  <si>
-    <t>A diversity of flower types lets you create interesting, abundant mixed bouquets that keep subscribers excited week after week.</t>
-  </si>
-  <si>
-    <t>Without enough variety of floral ingredients, mixed bouquets can look lackluster and lead to subscriber drop-offs.</t>
-  </si>
-  <si>
-    <t>Subscriptions generally rely heavily on mixed bouquets. To do them well, you need a steady flow of diverse ingredients across the season.</t>
-  </si>
-  <si>
-    <t>Strong planning and succession planting ensure you always have enough stems to fulfill weekly commitments without scrambling.</t>
-  </si>
-  <si>
-    <t>Without reliable production, you risk gaps in your ability to produce bouquets on-schedule. Even when customers are understanding, the extra time spent managing cancellations, rescheduling, and notifications eats into both your profits and your focus.</t>
-  </si>
-  <si>
-    <t>Good design skills keep mixed bouquets looking polished and exciting, even with the same core crops from week to week.</t>
-  </si>
-  <si>
-    <t>Subscription customers are buying your bouquets sight-unseen, and so are placing trust in your ability to create beautiful bouquets week after week.</t>
-  </si>
-  <si>
-    <t>Weak designs can make bouquets feel repetitive or amateur, which may lead subscribers to question the value of continuing.</t>
-  </si>
-  <si>
-    <t>Strong time management means you can harvest, design, and deliver on schedule every week.</t>
-  </si>
-  <si>
-    <t>Poor organization makes subscription weeks stressful and increases the risk of mistakes like late deliveries or missed bouquets.</t>
-  </si>
-  <si>
-    <t>Subscriptions impose fixed weekly deadlines, often with little flexibility. Organization and time discipline are crucial for consistent fulfillment.</t>
-  </si>
-  <si>
-    <t>Subscriptions live or die on customer trust. Clear communication, quick responses, and problem-solving are essential for long-term retention.</t>
-  </si>
-  <si>
-    <t>Without attentive service, small issues like a missed bouquet or unclear pickup instructions can lead to cancellations.</t>
-  </si>
-  <si>
-    <t>Strong customer service skills help you handle delivery issues, substitutions, and questions smoothly, keeping subscribers happy and loyal.</t>
-  </si>
-  <si>
     <t>Unlike a farmers market that provides built-in traffic, a farm stand depends on your ability to attract visitors to your location.</t>
   </si>
   <si>
@@ -877,6 +733,150 @@
   </si>
   <si>
     <t>Strong color awareness ensures you grow and supply palettes that match florist demand; making you their go-to source for locally grown flowers.</t>
+  </si>
+  <si>
+    <t>markets are built on direct interactions</t>
+  </si>
+  <si>
+    <t>strong customer service skills and sales ability help you build a loyal following, sell (and upsell) effectively, and position yourself for growth into other revenue streams</t>
+  </si>
+  <si>
+    <t>weaker customer service and sales skills make it easy to get overlooked in a busy market, with customers gravitating toward more engaging vendors</t>
+  </si>
+  <si>
+    <t>diverse crop offerings give you the ingredients needed to create abundant, eye-catching mixed bouquets that attract a wide range of buyers</t>
+  </si>
+  <si>
+    <t>limited crop diversity makes it hard to build mixed bouquets, leaving your booth looking sparse compared to other vendors</t>
+  </si>
+  <si>
+    <t>mixed bouquets are nearly required at farmers markets, and doing them well depends on having diverse ingredients</t>
+  </si>
+  <si>
+    <t>proximity to markets makes it easier to transport flowers, saving time and money, and reducing stress</t>
+  </si>
+  <si>
+    <t>being far from markets adds long drives and transport stress, cutting into profits and reducing farm time</t>
+  </si>
+  <si>
+    <t>time and transport costs directly affect profitability; the closer you are to a market, the stronger your bottom line</t>
+  </si>
+  <si>
+    <t>solid infrastructure like coolers, tents, and safe transport keeps flowers fresh, setup smooth, and you prepared each week</t>
+  </si>
+  <si>
+    <t>weak infrastructure leads to wilted flowers, chaotic setup, and stress before customers even arrive</t>
+  </si>
+  <si>
+    <t>transporting, storing, and displaying flowers is demanding; without infrastructure, quality and presentation suffer</t>
+  </si>
+  <si>
+    <t>careful crop planning and succession planting keep harvests steady, ensuring abundant stems every week for market bouquets</t>
+  </si>
+  <si>
+    <t>poor planning and failed successions cause harvests to come in flushes, leaving you short on product some weeks and unable to meet demand</t>
+  </si>
+  <si>
+    <t>consistent presence at market is critical to building loyal customers; when shoppers know you’ll be there every week with abundant offerings, they’ll seek out your booth</t>
+  </si>
+  <si>
+    <t>flexibility in your schedule that matches the market’s rhythm — including harvest, prep, and market day — makes weekly commitment possible</t>
+  </si>
+  <si>
+    <t>if the market’s schedule conflicts with immovable commitments, showing up consistently will be difficult or impossible</t>
+  </si>
+  <si>
+    <t>markets run on fixed days and times; success depends on aligning farm work and personal life to that schedule</t>
+  </si>
+  <si>
+    <t>strong design skills help build mixed bouquets that are beautiful, balanced, and irresistible on the market table</t>
+  </si>
+  <si>
+    <t>weaker design skills can make bouquets look awkward or less professional, making it harder to compete with other vendors</t>
+  </si>
+  <si>
+    <t>mixed bouquets are a core market product; design skill directly affects your ability to attract customers and keep them coming back</t>
+  </si>
+  <si>
+    <t>an outgoing, approachable personality helps connect with customers, build loyalty, and create a welcoming booth atmosphere</t>
+  </si>
+  <si>
+    <t>if social interaction is draining, markets may feel exhausting and limit your ability to engage effectively with buyers</t>
+  </si>
+  <si>
+    <t>markets are inherently social; success often depends as much on your presence and demeanor as on the flowers themselves</t>
+  </si>
+  <si>
+    <t>strong time management and organization let you juggle harvesting, bouquet-making, and market prep while arriving on time, fully prepared, and all set up before customers arrive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weaker time management and organization skills can create chaotic market days — forgotten supplies, rushed prep, or late arrival that can even cost you your spot </t>
+  </si>
+  <si>
+    <t>markets place firm demands on punctuality and preparedness; most have immovable weekly deadlines and strict rules about set-up times</t>
+  </si>
+  <si>
+    <t>strong customer service skills help handle delivery issues, substitutions, and questions smoothly, keeping subscribers happy and loyal</t>
+  </si>
+  <si>
+    <t>subscriptions live or die on customer trust; clear communication, quick responses, and problem-solving are essential for retention</t>
+  </si>
+  <si>
+    <t>good marketing skills help attract new subscribers, highlight the value of bouquets, and keep your subscriber list full</t>
+  </si>
+  <si>
+    <t>weak marketing capabilities may cause your subscriber list to stay small or fail to grow</t>
+  </si>
+  <si>
+    <t>unlike farmers markets, subscriptions require you to drive sign-ups yourself; marketing is essential for attracting customers</t>
+  </si>
+  <si>
+    <t>leveraging personal networks makes it easier to find first subscribers, as friends, colleagues, and local contacts are often earliest supporters</t>
+  </si>
+  <si>
+    <t>without strong personal connections, launching a subscription can be slow and momentum harder to build</t>
+  </si>
+  <si>
+    <t>many subscription programs start small and grow by word of mouth; a farmer’s existing relationships often determine how quickly a list fills</t>
+  </si>
+  <si>
+    <t>inattentive service means issues like a missed bouquet or unclear pickup instructions can lead to cancellations</t>
+  </si>
+  <si>
+    <t>diverse flower types let you create abundant mixed bouquets that keep subscribers excited week after week</t>
+  </si>
+  <si>
+    <t>limited variety of floral ingredients makes bouquets look lackluster and can lead to subscriber drop-offs</t>
+  </si>
+  <si>
+    <t>subscriptions rely heavily on mixed bouquets; doing them well requires a steady flow of diverse ingredients</t>
+  </si>
+  <si>
+    <t>strong planning and succession planting ensure enough stems each week to meet commitments without scrambling</t>
+  </si>
+  <si>
+    <t>unreliable production risks gaps in weekly deliveries; managing cancellations and reschedules cuts into profits and focus</t>
+  </si>
+  <si>
+    <t>subscriptions are a promise; predictability underpins the model and reduces risk of cancellations or reschedules</t>
+  </si>
+  <si>
+    <t>strong design skills keep mixed bouquets polished and exciting and help you build them quickly</t>
+  </si>
+  <si>
+    <t>subscription customers buy bouquets sight-unseen, trusting your ability to create beautiful designs each week</t>
+  </si>
+  <si>
+    <t>weak designs make bouquets feel repetitive or amateur, leading subscribers to question the value of continuing</t>
+  </si>
+  <si>
+    <t>strong time management ensures you can harvest, design, and deliver on schedule every week and organization skills are key to pulling off efficient delivery schedules</t>
+  </si>
+  <si>
+    <t>poor time management and organization makes subscription weeks stressful and increases the risk of late deliveries or missed bouquets</t>
+  </si>
+  <si>
+    <t>subscriptions assume fixed weekly deadlines with limited flexibility; organization and discipline are crucial for consistency</t>
   </si>
 </sst>
 </file>
@@ -978,7 +978,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1041,9 +1041,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2811,7 +2808,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>26</v>
       </c>
@@ -2907,7 +2904,7 @@
         <v>Proximity to Customers, Product Diversity, Floral Design</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>28</v>
       </c>
@@ -2955,7 +2952,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>29</v>
       </c>
@@ -3243,7 +3240,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
@@ -3291,7 +3288,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -3339,7 +3336,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>37</v>
       </c>
@@ -3387,7 +3384,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>38</v>
       </c>
@@ -3435,7 +3432,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
@@ -3483,7 +3480,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>40</v>
       </c>
@@ -3531,7 +3528,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>41</v>
       </c>
@@ -3627,7 +3624,7 @@
         <v>Product Diversity, Floral Design</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>43</v>
       </c>
@@ -4466,8 +4463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EBBEDC-5414-B442-BDB4-EC1529FD0ACE}">
   <dimension ref="A1:G343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4505,7 +4502,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>130</v>
       </c>
@@ -4519,13 +4516,13 @@
         <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>158</v>
+        <v>224</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>157</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -4570,7 +4567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>130</v>
       </c>
@@ -4584,13 +4581,13 @@
         <v>4</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>159</v>
+        <v>228</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>160</v>
+        <v>229</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>161</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4635,7 +4632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>130</v>
       </c>
@@ -4649,13 +4646,13 @@
         <v>5</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>163</v>
+        <v>225</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>162</v>
+        <v>226</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>164</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4686,16 +4683,16 @@
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>166</v>
+        <v>231</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>165</v>
+        <v>232</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>130</v>
       </c>
@@ -4709,13 +4706,13 @@
         <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>169</v>
+        <v>234</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>170</v>
+        <v>235</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>168</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -4732,13 +4729,13 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>172</v>
+        <v>237</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>171</v>
+        <v>238</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>173</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -4755,7 +4752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>130</v>
       </c>
@@ -4769,13 +4766,13 @@
         <v>4</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>175</v>
+        <v>241</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>174</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -4806,13 +4803,13 @@
         <v>5</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>178</v>
+        <v>244</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>179</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -4829,7 +4826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>130</v>
       </c>
@@ -4843,82 +4840,82 @@
         <v>5</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>180</v>
+        <v>246</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>181</v>
+        <v>247</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>182</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>152</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="14">
-        <v>4</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>205</v>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>204</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="14">
-        <v>5</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>184</v>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>185</v>
+        <v>252</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>183</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>152</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="14">
-        <v>4</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>188</v>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -4949,13 +4946,13 @@
         <v>4</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>191</v>
+        <v>158</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -5000,7 +4997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -5014,13 +5011,13 @@
         <v>5</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>193</v>
+        <v>258</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>194</v>
+        <v>259</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>195</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -5051,7 +5048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>27</v>
       </c>
@@ -5065,13 +5062,13 @@
         <v>4</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>196</v>
+        <v>261</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>197</v>
+        <v>262</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>192</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -5102,7 +5099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>27</v>
       </c>
@@ -5116,13 +5113,13 @@
         <v>4</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>198</v>
+        <v>264</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>200</v>
+        <v>266</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>199</v>
+        <v>265</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -5181,13 +5178,13 @@
         <v>4</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>201</v>
+        <v>267</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>202</v>
+        <v>268</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>203</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -5218,13 +5215,13 @@
         <v>5</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>209</v>
+        <v>161</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>208</v>
+        <v>160</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>207</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -5241,13 +5238,13 @@
         <v>4</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F42" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="G42" s="23" t="s">
-        <v>212</v>
+        <v>162</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -5263,7 +5260,6 @@
       <c r="D43" s="14">
         <v>1</v>
       </c>
-      <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
@@ -5279,13 +5275,13 @@
         <v>5</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>214</v>
+        <v>166</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>215</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -5302,13 +5298,13 @@
         <v>4</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>218</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -5324,7 +5320,6 @@
       <c r="D46" s="14">
         <v>3</v>
       </c>
-      <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
@@ -5340,13 +5335,13 @@
         <v>4</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>219</v>
+        <v>171</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>220</v>
+        <v>172</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>221</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -5363,13 +5358,13 @@
         <v>4</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>225</v>
+        <v>177</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>226</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -5456,13 +5451,13 @@
         <v>4</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>222</v>
+        <v>174</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>223</v>
+        <v>175</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -5535,13 +5530,13 @@
         <v>4</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>230</v>
+        <v>182</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>229</v>
+        <v>181</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>228</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -5558,13 +5553,13 @@
         <v>5</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>233</v>
+        <v>185</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>232</v>
+        <v>184</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>231</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -5609,13 +5604,13 @@
         <v>4</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>234</v>
+        <v>186</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>236</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -5674,13 +5669,13 @@
         <v>5</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>237</v>
+        <v>189</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>238</v>
+        <v>190</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>239</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -5739,13 +5734,13 @@
         <v>4</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>248</v>
+        <v>200</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>247</v>
+        <v>199</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -5776,13 +5771,13 @@
         <v>5</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>240</v>
+        <v>192</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>241</v>
+        <v>193</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>242</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -5799,13 +5794,13 @@
         <v>4</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>243</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -5878,13 +5873,13 @@
         <v>5</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>251</v>
+        <v>203</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>250</v>
+        <v>202</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -5985,13 +5980,13 @@
         <v>4</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>253</v>
+        <v>205</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>254</v>
+        <v>206</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>252</v>
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -6036,13 +6031,13 @@
         <v>4</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -6087,13 +6082,13 @@
         <v>4</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>260</v>
+        <v>212</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>259</v>
+        <v>211</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>258</v>
+        <v>210</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -6306,13 +6301,13 @@
         <v>4</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>263</v>
+        <v>215</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>262</v>
+        <v>214</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>261</v>
+        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -6329,13 +6324,13 @@
         <v>4</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>266</v>
+        <v>218</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>265</v>
+        <v>217</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>264</v>
+        <v>216</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -6394,13 +6389,13 @@
         <v>4</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>269</v>
+        <v>221</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>267</v>
+        <v>219</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>268</v>
+        <v>220</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed indentation error causing narrative section not to work
</commit_message>
<xml_diff>
--- a/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
+++ b/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Downloads/rsc-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB4E07A-0D20-6D4F-A435-475FA4986C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F50901-3CC7-874F-8CA3-1ED8C2FCB765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -738,30 +738,9 @@
     <t>markets are built on direct interactions</t>
   </si>
   <si>
-    <t>strong customer service skills and sales ability help you build a loyal following, sell (and upsell) effectively, and position yourself for growth into other revenue streams</t>
-  </si>
-  <si>
-    <t>weaker customer service and sales skills make it easy to get overlooked in a busy market, with customers gravitating toward more engaging vendors</t>
-  </si>
-  <si>
-    <t>diverse crop offerings give you the ingredients needed to create abundant, eye-catching mixed bouquets that attract a wide range of buyers</t>
-  </si>
-  <si>
-    <t>limited crop diversity makes it hard to build mixed bouquets, leaving your booth looking sparse compared to other vendors</t>
-  </si>
-  <si>
     <t>mixed bouquets are nearly required at farmers markets, and doing them well depends on having diverse ingredients</t>
   </si>
   <si>
-    <t>proximity to markets makes it easier to transport flowers, saving time and money, and reducing stress</t>
-  </si>
-  <si>
-    <t>being far from markets adds long drives and transport stress, cutting into profits and reducing farm time</t>
-  </si>
-  <si>
-    <t>time and transport costs directly affect profitability; the closer you are to a market, the stronger your bottom line</t>
-  </si>
-  <si>
     <t>solid infrastructure like coolers, tents, and safe transport keeps flowers fresh, setup smooth, and you prepared each week</t>
   </si>
   <si>
@@ -877,6 +856,27 @@
   </si>
   <si>
     <t>subscriptions assume fixed weekly deadlines with limited flexibility; organization and discipline are crucial for consistency</t>
+  </si>
+  <si>
+    <t>your strong customer service skills and sales ability help you build a loyal following, sell (and upsell) effectively, and position yourself for growth into other revenue streams</t>
+  </si>
+  <si>
+    <t>your weaker customer service and sales skills make it easy to get overlooked in a busy market, with customers gravitating toward more engaging vendors</t>
+  </si>
+  <si>
+    <t>your proximity to markets makes it easier to transport flowers, saving time and money, and reducing stress</t>
+  </si>
+  <si>
+    <t>time and transport costs directly affect profitability</t>
+  </si>
+  <si>
+    <t>your diverse crop offerings give you the ingredients needed to create abundant, eye-catching mixed bouquets that attract a wide range of buyers</t>
+  </si>
+  <si>
+    <t>your limited crop diversity makes it hard to build mixed bouquets, leaving your booth looking sparse compared to other vendors</t>
+  </si>
+  <si>
+    <t>your distance from markets means long drives and transport stress</t>
   </si>
 </sst>
 </file>
@@ -4463,8 +4463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EBBEDC-5414-B442-BDB4-EC1529FD0ACE}">
   <dimension ref="A1:G343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4516,10 +4516,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>222</v>
@@ -4581,13 +4581,13 @@
         <v>4</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>228</v>
+        <v>265</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4632,7 +4632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>130</v>
       </c>
@@ -4646,13 +4646,13 @@
         <v>5</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>225</v>
+        <v>267</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>226</v>
+        <v>268</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4683,13 +4683,13 @@
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -4706,13 +4706,13 @@
         <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -4729,13 +4729,13 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -4766,13 +4766,13 @@
         <v>4</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -4803,13 +4803,13 @@
         <v>5</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -4840,13 +4840,13 @@
         <v>5</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -4863,13 +4863,13 @@
         <v>4</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -4886,13 +4886,13 @@
         <v>5</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -4909,13 +4909,13 @@
         <v>4</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -5011,13 +5011,13 @@
         <v>5</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -5062,13 +5062,13 @@
         <v>4</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -5113,13 +5113,13 @@
         <v>4</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -5178,13 +5178,13 @@
         <v>4</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added code to handle edge cases where all user scores related to the channel are high or low
</commit_message>
<xml_diff>
--- a/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
+++ b/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Downloads/rsc-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F50901-3CC7-874F-8CA3-1ED8C2FCB765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975EFA93-1E37-4240-B47A-6DFDD790C531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -858,9 +858,6 @@
     <t>subscriptions assume fixed weekly deadlines with limited flexibility; organization and discipline are crucial for consistency</t>
   </si>
   <si>
-    <t>your strong customer service skills and sales ability help you build a loyal following, sell (and upsell) effectively, and position yourself for growth into other revenue streams</t>
-  </si>
-  <si>
     <t>your weaker customer service and sales skills make it easy to get overlooked in a busy market, with customers gravitating toward more engaging vendors</t>
   </si>
   <si>
@@ -877,6 +874,9 @@
   </si>
   <si>
     <t>your distance from markets means long drives and transport stress</t>
+  </si>
+  <si>
+    <t>your strong customer service skills and sales ability will help you build a loyal following, sell (and upsell) effectively, and position yourself for growth into other revenue streams</t>
   </si>
 </sst>
 </file>
@@ -4464,7 +4464,7 @@
   <dimension ref="A1:G343"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4516,10 +4516,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>264</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>222</v>
@@ -4581,13 +4581,13 @@
         <v>4</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4646,10 +4646,10 @@
         <v>5</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>268</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>223</v>

</xml_diff>

<commit_message>
added normalization of scores so user's weighted average is divided by the best possible wieghted average for the channel
</commit_message>
<xml_diff>
--- a/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
+++ b/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Downloads/rsc-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52D000E-139F-0B43-A9E4-C695D221C895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2747B6-AD71-1F4F-A405-17A6D209C3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1913,7 +1913,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2372,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="N8" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O8" s="7">
         <v>1</v>
@@ -2431,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O9" s="7">
         <v>1</v>
@@ -2726,7 +2726,7 @@
         <v>5</v>
       </c>
       <c r="N14" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O14" s="7">
         <v>5</v>
@@ -4806,8 +4806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EBBEDC-5414-B442-BDB4-EC1529FD0ACE}">
   <dimension ref="A1:G343"/>
   <sheetViews>
-    <sheetView topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="G254" sqref="G254"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changed max factors so it's looking at only those factors that have an adjusted weight or 8 or greater (excel spreadsheet weight scores of 4 or greater)
</commit_message>
<xml_diff>
--- a/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
+++ b/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Downloads/rsc-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2747B6-AD71-1F4F-A405-17A6D209C3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D9D0E4-DF4D-354D-B8CC-FEAFD9D173B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1913,7 +1913,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2640,7 +2640,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="7">
         <v>4</v>

</xml_diff>

<commit_message>
not sure what these latest changes are???
</commit_message>
<xml_diff>
--- a/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
+++ b/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Downloads/rsc-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE979989-782B-A74A-B140-A1A2244909D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6F6CAE-0937-1541-8909-C79DDAEA4018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="493">
   <si>
     <t>Section</t>
   </si>
@@ -1186,6 +1186,366 @@
   </si>
   <si>
     <t>Do you have the flexibility to operate without restrictive zoning laws, HOA rules, or permitting requirements that might limit hosting events, building structures, or selling directly from your farm?</t>
+  </si>
+  <si>
+    <t>strong customer service and sales skills help you book repeat clients, manage expectations, and respond smoothly to requests</t>
+  </si>
+  <si>
+    <t>weak customer service and sales ability makes it harder to secure contracts or maintain long-term client relationships</t>
+  </si>
+  <si>
+    <t>events often depend on reputation and repeat business; service and sales skills directly influence bookings and retention</t>
+  </si>
+  <si>
+    <t>effective marketing helps you showcase your work and connect with organizations looking for floral services</t>
+  </si>
+  <si>
+    <t>weak marketing presence limits visibility and reduces opportunities to pitch for event contracts</t>
+  </si>
+  <si>
+    <t>organizations often plan events months in advance; consistent marketing ensures you’re on their radar at the right time</t>
+  </si>
+  <si>
+    <t>lack of networking may make it harder to learn about opportunities or get your foot in the door when making cold inquiries</t>
+  </si>
+  <si>
+    <t>relationships drive event work; being known and trusted in professional circles is helpful for access</t>
+  </si>
+  <si>
+    <t>a strong professional network can help connect you with planners, venues, and organizations that regularly need floral design</t>
+  </si>
+  <si>
+    <t>diverse crops allow you to create designs for varied event themes and client needs</t>
+  </si>
+  <si>
+    <t>limited product diversity restricts your ability to match palettes or styles for different organizations and different types of events</t>
+  </si>
+  <si>
+    <t>events may require anything from small arrangements to large installations; diversity of floral materials ensures you have all of the ingredients needed to make beautiful designs</t>
+  </si>
+  <si>
+    <t>reliable infrastructure like coolers, vehicles, and staff capacity ensures flowers arrive fresh and setups run smoothly</t>
+  </si>
+  <si>
+    <t>weak infrastructure risks wilted flowers, delayed setups, or chaotic delivery logistics</t>
+  </si>
+  <si>
+    <t>events often require large orders delivered on strict timelines; infrastructure is essential for professional execution</t>
+  </si>
+  <si>
+    <t>unpredictable supply undermines your ability to meet client expectations and deadlines</t>
+  </si>
+  <si>
+    <t>consistent crop planning and effective succession plantings allow you to promise and deliver event orders with confidence</t>
+  </si>
+  <si>
+    <t>organizations expect guaranteed delivery and bookings may be made well in advance of the event; crop predictability is key to being able to accurately describe what you will be able to provide on the day of the event</t>
+  </si>
+  <si>
+    <t>events are often fixed to specific dates and times; flexibility ensures you can say yes and deliver reliably</t>
+  </si>
+  <si>
+    <t>your ability to adapt to the clients' schedule ensures you can book more events, which drives revenue higher</t>
+  </si>
+  <si>
+    <t>conflicting commitments make it difficult to meet event timelines and may cause you to have to pass on opportunities</t>
+  </si>
+  <si>
+    <t>strong financial resources allow you to cover upfront costs for large orders or staffing until payment arrives</t>
+  </si>
+  <si>
+    <t>events often require investment before payment; financial resources give you the ability to commit confidently</t>
+  </si>
+  <si>
+    <t>limited financial reserves create cash-flow stress and may make it harder to take on bigger contracts</t>
+  </si>
+  <si>
+    <t>strong design skills let you create professional arrangements that elevate events and impress clients</t>
+  </si>
+  <si>
+    <t>weak design skills lead to underwhelming displays that may prevent repeat business</t>
+  </si>
+  <si>
+    <t>organizations hire florists to enhance their events; design quality directly affects satisfaction and reputation</t>
+  </si>
+  <si>
+    <t>high stress tolerance helps you manage tight timelines, large orders, and event-day pressures</t>
+  </si>
+  <si>
+    <t>low stress tolerance can make event work overwhelming and increase the chance of mistakes</t>
+  </si>
+  <si>
+    <t>events often involve last-minute changes and high client expectations; stress management is essential</t>
+  </si>
+  <si>
+    <t>poor organization risks late arrivals, forgotten items, or rushed setups</t>
+  </si>
+  <si>
+    <t>events involve many moving parts on fixed schedules; time discipline and organization are critical to success</t>
+  </si>
+  <si>
+    <t>strong organization and time management ensures smooth coordination from booking to harvest to design to delivery and setup</t>
+  </si>
+  <si>
+    <t>a strong eye for color ensures you can match palettes to client branding, event themes, or seasonal styles</t>
+  </si>
+  <si>
+    <t>color accuracy is especially important for organizations that prioritize branding or consistent visual presentation</t>
+  </si>
+  <si>
+    <t>weak color comprehension risks arrangements that don’t align with event aesthetics or client expectations</t>
+  </si>
+  <si>
+    <t>strong professional relationships with chefs, managers, and hospitality staff help secure and maintain contracts</t>
+  </si>
+  <si>
+    <t>hotel and restaurant work is built on relationships; trusted connections often determine who gets the contract</t>
+  </si>
+  <si>
+    <t>long travel distances increase costs, stress, and the risk of damaged product</t>
+  </si>
+  <si>
+    <t>lack of networking limits opportunities and may make it harder to get connected with potential clients</t>
+  </si>
+  <si>
+    <t>hospitality accounts require frequent, reliable delivery, including touch-ups and refreshing of arrangements; proximity directly affects profitability</t>
+  </si>
+  <si>
+    <t>being located near hotels and restaurants makes deliveries efficient and makes repeat trips less taxing on bottom-line profits</t>
+  </si>
+  <si>
+    <t>limited diversity restricts your ability to provide consistent variety and may make your work feel repetitive</t>
+  </si>
+  <si>
+    <t>diverse crop offerings allow you to meet varied design needs, from simple restaurant table bud vases to large hotel lobby arrangements</t>
+  </si>
+  <si>
+    <t>hospitality clients expect fresh, changing arrangements; a diversity of floral materials is key to being able to create beautiful arrangements</t>
+  </si>
+  <si>
+    <t>weak infrastructure risks wilted product, missed drop-offs, or logistical breakdowns</t>
+  </si>
+  <si>
+    <t>hospitality contracts involve frequent, scheduled deliveries; infrastructure underpins quality and reliability</t>
+  </si>
+  <si>
+    <t>reliable infrastructure like coolers, vehicles, and storage for hardgoods ensures you can deliver quality product with high efficiency</t>
+  </si>
+  <si>
+    <t>rigid schedules make it difficult to meet hospitality delivery windows and may cause lost contracts</t>
+  </si>
+  <si>
+    <t>flexible scheduling allows you to accommodate the customers' desired delivery windows</t>
+  </si>
+  <si>
+    <t>these clients often require deliveries on regular, set schedules; flexibility is crucial to meeting their needs</t>
+  </si>
+  <si>
+    <t>strong financial resources allow you to cover upfront costs for supplies and labor until regular payments are received</t>
+  </si>
+  <si>
+    <t>limited financial reserves make it difficult to handle delays or invest in capacity growth</t>
+  </si>
+  <si>
+    <t>hospitality contracts are usually stable but may pay on net terms; financial resources help bridge gaps</t>
+  </si>
+  <si>
+    <t>strong design skills let you create arrangements that enhance the ambiance and align with brand aesthetics</t>
+  </si>
+  <si>
+    <t>weak design skills result in uninspired arrangements that fail to impress staff or guests</t>
+  </si>
+  <si>
+    <t>hotels and restaurants use flowers to reinforce their brand; design quality directly affects client satisfaction</t>
+  </si>
+  <si>
+    <t>strong organization ensures consistent harvest, design, and delivery to meet weekly hospitality schedules</t>
+  </si>
+  <si>
+    <t>poor time management risks late or missed deliveries, eroding client trust</t>
+  </si>
+  <si>
+    <t>hospitality clients expect precise, regular delivery; time discipline is critical for retaining contracts</t>
+  </si>
+  <si>
+    <t>strong customer service and sales skills help you welcome guests, answer questions, and encourage purchases beyond admission fees</t>
+  </si>
+  <si>
+    <t>weak service or sales ability may leave visitors feeling unsupported or reduce upsell opportunities</t>
+  </si>
+  <si>
+    <t>PYO events depend on hospitality and interaction; customer service directly influences satisfaction and repeat visits</t>
+  </si>
+  <si>
+    <t>effective marketing helps you attract families, groups, and visitors to your farm</t>
+  </si>
+  <si>
+    <t>weak marketing presence makes it hard to bring in enough participants to cover event costs</t>
+  </si>
+  <si>
+    <t>PYO events rely on visitor turnout; strong marketing drives attendance and revenue</t>
+  </si>
+  <si>
+    <t>strong visual appeal and immersive experiences make your farm a destination people want to visit</t>
+  </si>
+  <si>
+    <t>PYO events are as much about the experience as the flowers; aesthetics shape customer enjoyment</t>
+  </si>
+  <si>
+    <t>lack of visual or experiential appeal may make events feel underwhelming and discourages repeat visits</t>
+  </si>
+  <si>
+    <t>offering amenities like parking, restrooms, and shade keeps guests comfortable and increases satisfaction</t>
+  </si>
+  <si>
+    <t>lack of amenities creates frustration and shortens visits, reducing overall sales</t>
+  </si>
+  <si>
+    <t>PYO events are family-friendly experiences; basic amenities make them accessible and enjoyable</t>
+  </si>
+  <si>
+    <t>operating in an area with few restrictions allows you to host events easily and frequently</t>
+  </si>
+  <si>
+    <t>local rules often determine whether you can legally and affordably host PYO events</t>
+  </si>
+  <si>
+    <t>strict regulations or zoning barriers make events harder or impossible to run and may limit attendance</t>
+  </si>
+  <si>
+    <t>high production levels ensure there are enough flowers for visitors to pick throughout the event</t>
+  </si>
+  <si>
+    <t>low production creates scarcity, disappointing visitors and reducing revenue</t>
+  </si>
+  <si>
+    <t>PYO events require abundance; guests expect plentiful flowers to choose from</t>
+  </si>
+  <si>
+    <t>high stress tolerance helps you handle unpredictable weather, visitor behavior, and event logistics</t>
+  </si>
+  <si>
+    <t>low stress tolerance can make events overwhelming</t>
+  </si>
+  <si>
+    <t>PYO events means having strangers on your property and involves many variables outside your control; resilience is helpful for success</t>
+  </si>
+  <si>
+    <t>weak service or sales ability can make workshops feel flat, leaving participants less likely to return</t>
+  </si>
+  <si>
+    <t>strong customer service and sales skills help you engage participants, answer questions, and encourage additional purchases and return visits for future workshops</t>
+  </si>
+  <si>
+    <t>workshops are built on interaction and trust; customer engagement and attention to serving their needs directly influences participant experience and repeat business</t>
+  </si>
+  <si>
+    <t>effective marketing helps you fill seats and promote workshops as special experiences</t>
+  </si>
+  <si>
+    <t>weak marketing presence makes it difficult to attract enough participants to cover costs</t>
+  </si>
+  <si>
+    <t>workshops depend on drawing an audience; strong marketing drives attendance and profitability</t>
+  </si>
+  <si>
+    <t>an attractive setting and engaging atmosphere make workshops feel special and worth the price</t>
+  </si>
+  <si>
+    <t>lack of appeal in the environment or experience reduces participant satisfaction and word-of-mouth</t>
+  </si>
+  <si>
+    <t>workshops are experiences as much as educational events; your farm's aesthetics help shape how memorable they are</t>
+  </si>
+  <si>
+    <t>offering amenities like parking, restrooms, and comfortable seating keeps participants relaxed and focused</t>
+  </si>
+  <si>
+    <t>lack of amenities creates discomfort and detracts from the learning experience</t>
+  </si>
+  <si>
+    <t>workshops require basic comfort to support a positive participant experience</t>
+  </si>
+  <si>
+    <t>operating in an area with minimal restrictions makes it easy to host workshops on your farm</t>
+  </si>
+  <si>
+    <t>regulations can determine whether workshops are feasible and profitable on your property</t>
+  </si>
+  <si>
+    <t>strict local rules or permits may complicate hosting events and add costs or significant restrictions</t>
+  </si>
+  <si>
+    <t>diverse flower offerings allow you to teach different design techniques and keep classes interesting</t>
+  </si>
+  <si>
+    <t>limited variety makes workshops repetitive and less inspiring for participants</t>
+  </si>
+  <si>
+    <t>product diversity gives participants a richer, more engaging experience and increases perceived value</t>
+  </si>
+  <si>
+    <t>strong design skills allow you to confidently teach techniques and demonstrate professional-quality results</t>
+  </si>
+  <si>
+    <t>workshops rely on teaching and inspiration; design skill is central to participant confidence in your expertise</t>
+  </si>
+  <si>
+    <t>weak design skills can potentially undermine your authority as an instructor and can leave participants dissatisfied</t>
+  </si>
+  <si>
+    <t>an outgoing, approachable personality helps you connect with participants and create an enjoyable group dynamic</t>
+  </si>
+  <si>
+    <t>workshops are social learning experiences; personality plays a big role in participant enjoyment</t>
+  </si>
+  <si>
+    <t>introversion or discomfort in social settings can make workshops feel stiff or less engaging, and/or drain you of energy</t>
+  </si>
+  <si>
+    <t>high stress tolerance helps you manage live teaching, event logistics, and unexpected participant needs</t>
+  </si>
+  <si>
+    <t>low stress tolerance can make workshop delivery overwhelming and prone to mistakes</t>
+  </si>
+  <si>
+    <t>workshops involve teaching in real time and often involve having strangers on your property; resilience is essential for smooth execution</t>
+  </si>
+  <si>
+    <t>effective marketing helps you reach photographers, families, and couples looking for scenic backdrops</t>
+  </si>
+  <si>
+    <t>photography venues rely on visibility and word-of-mouth; strong marketing ensures steady interest and rentals</t>
+  </si>
+  <si>
+    <t>weak marketing presence makes it difficult to attract bookings</t>
+  </si>
+  <si>
+    <t>strong visual appeal makes your farm an attractive backdrop for photos and increases bookings</t>
+  </si>
+  <si>
+    <t>lack of aesthetic appeal reduces demand and limits the types of shoots your venue can host</t>
+  </si>
+  <si>
+    <t>photography venues succeed on appearance; visual quality directly influences desirability</t>
+  </si>
+  <si>
+    <t>lack of amenities creates inconvenience and reduces the professionalism of the experience</t>
+  </si>
+  <si>
+    <t>photography clients expect basic comfort and ease of use; amenities enhance satisfaction and repeat business</t>
+  </si>
+  <si>
+    <t>offering amenities like parking, changing areas, and restrooms makes sessions more comfortable for clients and photographers</t>
+  </si>
+  <si>
+    <t>low stress tolerance can make client management or sudden changes overwhelming</t>
+  </si>
+  <si>
+    <t>photography venues involve giving access to your farm to strangers</t>
+  </si>
+  <si>
+    <t>high stress tolerance helps you manage unpredictable weather, scheduling conflicts, and other variables that may arise with ease</t>
   </si>
 </sst>
 </file>
@@ -1913,7 +2273,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2269,7 +2629,7 @@
         <v>3</v>
       </c>
       <c r="S6" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -4107,7 +4467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4685398-D085-6B47-BDBF-4D7FCE78162F}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -4806,8 +5166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EBBEDC-5414-B442-BDB4-EC1529FD0ACE}">
   <dimension ref="A1:G343"/>
   <sheetViews>
-    <sheetView topLeftCell="A243" workbookViewId="0">
-      <selection activeCell="E249" sqref="E249"/>
+    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="F346" sqref="F346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8993,7 +9353,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="249" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A249" s="23" t="s">
         <v>141</v>
       </c>
@@ -9004,13 +9364,19 @@
         <v>7</v>
       </c>
       <c r="D249" s="24">
-        <v>4</v>
-      </c>
-      <c r="E249" s="25"/>
-      <c r="F249" s="25"/>
-      <c r="G249" s="25"/>
-    </row>
-    <row r="250" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E249" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="F249" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="G249" s="25" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A250" s="23" t="s">
         <v>141</v>
       </c>
@@ -9023,9 +9389,15 @@
       <c r="D250" s="24">
         <v>4</v>
       </c>
-      <c r="E250" s="25"/>
-      <c r="F250" s="25"/>
-      <c r="G250" s="25"/>
+      <c r="E250" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="F250" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="G250" s="25" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
@@ -9041,7 +9413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A252" s="23" t="s">
         <v>141</v>
       </c>
@@ -9054,9 +9426,15 @@
       <c r="D252" s="24">
         <v>4</v>
       </c>
-      <c r="E252" s="25"/>
-      <c r="F252" s="25"/>
-      <c r="G252" s="25"/>
+      <c r="E252" s="25" t="s">
+        <v>381</v>
+      </c>
+      <c r="F252" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="G252" s="25" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
@@ -9114,7 +9492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:7" s="23" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A257" s="23" t="s">
         <v>141</v>
       </c>
@@ -9127,9 +9505,15 @@
       <c r="D257" s="24">
         <v>5</v>
       </c>
-      <c r="E257" s="25"/>
-      <c r="F257" s="25"/>
-      <c r="G257" s="25"/>
+      <c r="E257" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="F257" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="G257" s="25" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
@@ -9145,7 +9529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A259" s="23" t="s">
         <v>141</v>
       </c>
@@ -9158,11 +9542,17 @@
       <c r="D259" s="24">
         <v>5</v>
       </c>
-      <c r="E259" s="25"/>
-      <c r="F259" s="25"/>
-      <c r="G259" s="25"/>
-    </row>
-    <row r="260" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E259" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="F259" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="G259" s="25" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" s="23" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A260" s="23" t="s">
         <v>141</v>
       </c>
@@ -9175,11 +9565,17 @@
       <c r="D260" s="24">
         <v>5</v>
       </c>
-      <c r="E260" s="25"/>
-      <c r="F260" s="25"/>
-      <c r="G260" s="25"/>
-    </row>
-    <row r="261" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E260" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="F260" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="G260" s="25" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A261" s="23" t="s">
         <v>141</v>
       </c>
@@ -9192,11 +9588,17 @@
       <c r="D261" s="24">
         <v>5</v>
       </c>
-      <c r="E261" s="25"/>
-      <c r="F261" s="25"/>
-      <c r="G261" s="25"/>
-    </row>
-    <row r="262" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E261" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="F261" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="G261" s="25" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A262" s="23" t="s">
         <v>141</v>
       </c>
@@ -9209,11 +9611,17 @@
       <c r="D262" s="24">
         <v>4</v>
       </c>
-      <c r="E262" s="25"/>
-      <c r="F262" s="25"/>
-      <c r="G262" s="25"/>
-    </row>
-    <row r="263" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E262" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="F262" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="G262" s="25" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A263" s="23" t="s">
         <v>141</v>
       </c>
@@ -9226,22 +9634,37 @@
       <c r="D263" s="24">
         <v>5</v>
       </c>
-      <c r="E263" s="25"/>
-      <c r="F263" s="25"/>
-      <c r="G263" s="25"/>
-    </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A264" s="3" t="s">
+      <c r="E263" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="F263" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="G263" s="25" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A264" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="B264" s="3" t="s">
+      <c r="B264" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C264" s="3" t="s">
+      <c r="C264" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D264" s="14">
-        <v>4</v>
+      <c r="D264" s="24">
+        <v>4</v>
+      </c>
+      <c r="E264" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="F264" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="G264" s="25" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.2">
@@ -9258,7 +9681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="266" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A266" s="23" t="s">
         <v>141</v>
       </c>
@@ -9271,11 +9694,17 @@
       <c r="D266" s="24">
         <v>4</v>
       </c>
-      <c r="E266" s="25"/>
-      <c r="F266" s="25"/>
-      <c r="G266" s="25"/>
-    </row>
-    <row r="267" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E266" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="F266" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="G266" s="25" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A267" s="23" t="s">
         <v>141</v>
       </c>
@@ -9288,9 +9717,15 @@
       <c r="D267" s="24">
         <v>5</v>
       </c>
-      <c r="E267" s="25"/>
-      <c r="F267" s="25"/>
-      <c r="G267" s="25"/>
+      <c r="E267" s="25" t="s">
+        <v>405</v>
+      </c>
+      <c r="F267" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="G267" s="25" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
@@ -9334,7 +9769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A271" s="23" t="s">
         <v>142</v>
       </c>
@@ -9347,11 +9782,17 @@
       <c r="D271" s="24">
         <v>4</v>
       </c>
-      <c r="E271" s="25"/>
-      <c r="F271" s="25"/>
-      <c r="G271" s="25"/>
-    </row>
-    <row r="272" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E271" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="F271" s="25" t="s">
+        <v>412</v>
+      </c>
+      <c r="G271" s="25" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" s="23" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A272" s="23" t="s">
         <v>142</v>
       </c>
@@ -9364,9 +9805,15 @@
       <c r="D272" s="24">
         <v>4</v>
       </c>
-      <c r="E272" s="25"/>
-      <c r="F272" s="25"/>
-      <c r="G272" s="25"/>
+      <c r="E272" s="25" t="s">
+        <v>414</v>
+      </c>
+      <c r="F272" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="G272" s="25" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
@@ -9410,7 +9857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:7" s="23" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A276" s="23" t="s">
         <v>142</v>
       </c>
@@ -9423,9 +9870,15 @@
       <c r="D276" s="24">
         <v>5</v>
       </c>
-      <c r="E276" s="25"/>
-      <c r="F276" s="25"/>
-      <c r="G276" s="25"/>
+      <c r="E276" s="25" t="s">
+        <v>416</v>
+      </c>
+      <c r="F276" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="G276" s="25" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
@@ -9441,7 +9894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A278" s="23" t="s">
         <v>142</v>
       </c>
@@ -9454,9 +9907,15 @@
       <c r="D278" s="24">
         <v>4</v>
       </c>
-      <c r="E278" s="25"/>
-      <c r="F278" s="25"/>
-      <c r="G278" s="25"/>
+      <c r="E278" s="25" t="s">
+        <v>420</v>
+      </c>
+      <c r="F278" s="25" t="s">
+        <v>418</v>
+      </c>
+      <c r="G278" s="25" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
@@ -9472,7 +9931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="280" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A280" s="23" t="s">
         <v>142</v>
       </c>
@@ -9485,11 +9944,17 @@
       <c r="D280" s="24">
         <v>4</v>
       </c>
-      <c r="E280" s="25"/>
-      <c r="F280" s="25"/>
-      <c r="G280" s="25"/>
-    </row>
-    <row r="281" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E280" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="F280" s="25" t="s">
+        <v>421</v>
+      </c>
+      <c r="G280" s="25" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A281" s="23" t="s">
         <v>142</v>
       </c>
@@ -9502,11 +9967,17 @@
       <c r="D281" s="24">
         <v>4</v>
       </c>
-      <c r="E281" s="25"/>
-      <c r="F281" s="25"/>
-      <c r="G281" s="25"/>
-    </row>
-    <row r="282" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E281" s="25" t="s">
+        <v>424</v>
+      </c>
+      <c r="F281" s="25" t="s">
+        <v>425</v>
+      </c>
+      <c r="G281" s="25" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A282" s="23" t="s">
         <v>142</v>
       </c>
@@ -9519,9 +9990,15 @@
       <c r="D282" s="24">
         <v>5</v>
       </c>
-      <c r="E282" s="25"/>
-      <c r="F282" s="25"/>
-      <c r="G282" s="25"/>
+      <c r="E282" s="25" t="s">
+        <v>427</v>
+      </c>
+      <c r="F282" s="25" t="s">
+        <v>428</v>
+      </c>
+      <c r="G282" s="25" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
@@ -9565,7 +10042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="286" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A286" s="23" t="s">
         <v>142</v>
       </c>
@@ -9578,11 +10055,17 @@
       <c r="D286" s="24">
         <v>5</v>
       </c>
-      <c r="E286" s="25"/>
-      <c r="F286" s="25"/>
-      <c r="G286" s="25"/>
-    </row>
-    <row r="287" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E286" s="25" t="s">
+        <v>430</v>
+      </c>
+      <c r="F286" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="G286" s="25" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A287" s="23" t="s">
         <v>143</v>
       </c>
@@ -9595,11 +10078,17 @@
       <c r="D287" s="24">
         <v>4</v>
       </c>
-      <c r="E287" s="25"/>
-      <c r="F287" s="25"/>
-      <c r="G287" s="25"/>
-    </row>
-    <row r="288" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E287" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="F287" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="G287" s="25" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" s="23" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A288" s="23" t="s">
         <v>143</v>
       </c>
@@ -9612,9 +10101,15 @@
       <c r="D288" s="24">
         <v>5</v>
       </c>
-      <c r="E288" s="25"/>
-      <c r="F288" s="25"/>
-      <c r="G288" s="25"/>
+      <c r="E288" s="25" t="s">
+        <v>436</v>
+      </c>
+      <c r="F288" s="25" t="s">
+        <v>437</v>
+      </c>
+      <c r="G288" s="25" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
@@ -9658,7 +10153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="292" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A292" s="23" t="s">
         <v>143</v>
       </c>
@@ -9671,11 +10166,17 @@
       <c r="D292" s="24">
         <v>4</v>
       </c>
-      <c r="E292" s="25"/>
-      <c r="F292" s="25"/>
-      <c r="G292" s="25"/>
-    </row>
-    <row r="293" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E292" s="25" t="s">
+        <v>439</v>
+      </c>
+      <c r="F292" s="25" t="s">
+        <v>441</v>
+      </c>
+      <c r="G292" s="25" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A293" s="23" t="s">
         <v>143</v>
       </c>
@@ -9688,11 +10189,17 @@
       <c r="D293" s="24">
         <v>5</v>
       </c>
-      <c r="E293" s="25"/>
-      <c r="F293" s="25"/>
-      <c r="G293" s="25"/>
-    </row>
-    <row r="294" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E293" s="25" t="s">
+        <v>442</v>
+      </c>
+      <c r="F293" s="25" t="s">
+        <v>443</v>
+      </c>
+      <c r="G293" s="25" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A294" s="23" t="s">
         <v>143</v>
       </c>
@@ -9705,9 +10212,15 @@
       <c r="D294" s="24">
         <v>5</v>
       </c>
-      <c r="E294" s="25"/>
-      <c r="F294" s="25"/>
-      <c r="G294" s="25"/>
+      <c r="E294" s="25" t="s">
+        <v>445</v>
+      </c>
+      <c r="F294" s="25" t="s">
+        <v>447</v>
+      </c>
+      <c r="G294" s="25" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
@@ -9723,7 +10236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="296" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:7" s="23" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A296" s="23" t="s">
         <v>143</v>
       </c>
@@ -9736,9 +10249,15 @@
       <c r="D296" s="24">
         <v>4</v>
       </c>
-      <c r="E296" s="25"/>
-      <c r="F296" s="25"/>
-      <c r="G296" s="25"/>
+      <c r="E296" s="25" t="s">
+        <v>448</v>
+      </c>
+      <c r="F296" s="25" t="s">
+        <v>449</v>
+      </c>
+      <c r="G296" s="25" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
@@ -9838,7 +10357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="304" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:7" s="23" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A304" s="23" t="s">
         <v>143</v>
       </c>
@@ -9851,9 +10370,15 @@
       <c r="D304" s="24">
         <v>4</v>
       </c>
-      <c r="E304" s="25"/>
-      <c r="F304" s="25"/>
-      <c r="G304" s="25"/>
+      <c r="E304" s="25" t="s">
+        <v>451</v>
+      </c>
+      <c r="F304" s="25" t="s">
+        <v>452</v>
+      </c>
+      <c r="G304" s="25" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
@@ -9869,7 +10394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="306" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:7" s="23" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A306" s="23" t="s">
         <v>42</v>
       </c>
@@ -9882,11 +10407,17 @@
       <c r="D306" s="24">
         <v>4</v>
       </c>
-      <c r="E306" s="25"/>
-      <c r="F306" s="25"/>
-      <c r="G306" s="25"/>
-    </row>
-    <row r="307" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E306" s="25" t="s">
+        <v>455</v>
+      </c>
+      <c r="F306" s="25" t="s">
+        <v>454</v>
+      </c>
+      <c r="G306" s="25" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A307" s="23" t="s">
         <v>42</v>
       </c>
@@ -9899,9 +10430,15 @@
       <c r="D307" s="24">
         <v>5</v>
       </c>
-      <c r="E307" s="25"/>
-      <c r="F307" s="25"/>
-      <c r="G307" s="25"/>
+      <c r="E307" s="25" t="s">
+        <v>457</v>
+      </c>
+      <c r="F307" s="25" t="s">
+        <v>458</v>
+      </c>
+      <c r="G307" s="25" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
@@ -9945,7 +10482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="311" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A311" s="23" t="s">
         <v>42</v>
       </c>
@@ -9958,11 +10495,17 @@
       <c r="D311" s="24">
         <v>4</v>
       </c>
-      <c r="E311" s="25"/>
-      <c r="F311" s="25"/>
-      <c r="G311" s="25"/>
-    </row>
-    <row r="312" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E311" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="F311" s="25" t="s">
+        <v>461</v>
+      </c>
+      <c r="G311" s="25" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A312" s="23" t="s">
         <v>42</v>
       </c>
@@ -9975,11 +10518,17 @@
       <c r="D312" s="24">
         <v>5</v>
       </c>
-      <c r="E312" s="25"/>
-      <c r="F312" s="25"/>
-      <c r="G312" s="25"/>
-    </row>
-    <row r="313" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E312" s="25" t="s">
+        <v>463</v>
+      </c>
+      <c r="F312" s="25" t="s">
+        <v>464</v>
+      </c>
+      <c r="G312" s="25" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A313" s="23" t="s">
         <v>42</v>
       </c>
@@ -9992,11 +10541,17 @@
       <c r="D313" s="24">
         <v>5</v>
       </c>
-      <c r="E313" s="25"/>
-      <c r="F313" s="25"/>
-      <c r="G313" s="25"/>
-    </row>
-    <row r="314" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E313" s="25" t="s">
+        <v>466</v>
+      </c>
+      <c r="F313" s="25" t="s">
+        <v>468</v>
+      </c>
+      <c r="G313" s="25" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A314" s="23" t="s">
         <v>42</v>
       </c>
@@ -10009,9 +10564,15 @@
       <c r="D314" s="24">
         <v>4</v>
       </c>
-      <c r="E314" s="25"/>
-      <c r="F314" s="25"/>
-      <c r="G314" s="25"/>
+      <c r="E314" s="25" t="s">
+        <v>469</v>
+      </c>
+      <c r="F314" s="25" t="s">
+        <v>470</v>
+      </c>
+      <c r="G314" s="25" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
@@ -10083,7 +10644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A320" s="23" t="s">
         <v>42</v>
       </c>
@@ -10096,9 +10657,15 @@
       <c r="D320" s="24">
         <v>5</v>
       </c>
-      <c r="E320" s="25"/>
-      <c r="F320" s="25"/>
-      <c r="G320" s="25"/>
+      <c r="E320" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="F320" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="G320" s="25" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="s">
@@ -10114,7 +10681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A322" s="23" t="s">
         <v>42</v>
       </c>
@@ -10127,11 +10694,17 @@
       <c r="D322" s="24">
         <v>5</v>
       </c>
-      <c r="E322" s="25"/>
-      <c r="F322" s="25"/>
-      <c r="G322" s="25"/>
-    </row>
-    <row r="323" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E322" s="25" t="s">
+        <v>475</v>
+      </c>
+      <c r="F322" s="25" t="s">
+        <v>477</v>
+      </c>
+      <c r="G322" s="25" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" s="23" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A323" s="23" t="s">
         <v>42</v>
       </c>
@@ -10144,9 +10717,15 @@
       <c r="D323" s="24">
         <v>4</v>
       </c>
-      <c r="E323" s="25"/>
-      <c r="F323" s="25"/>
-      <c r="G323" s="25"/>
+      <c r="E323" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="F323" s="25" t="s">
+        <v>479</v>
+      </c>
+      <c r="G323" s="25" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A324" s="3" t="s">
@@ -10176,18 +10755,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A326" s="3" t="s">
+    <row r="326" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A326" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="B326" s="3" t="s">
+      <c r="B326" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="C326" s="3" t="s">
+      <c r="C326" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D326" s="14">
-        <v>5</v>
+      <c r="D326" s="24">
+        <v>5</v>
+      </c>
+      <c r="E326" s="25" t="s">
+        <v>481</v>
+      </c>
+      <c r="F326" s="25" t="s">
+        <v>483</v>
+      </c>
+      <c r="G326" s="25" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.2">
@@ -10218,24 +10806,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="329" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A329" s="23" t="s">
+    <row r="329" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A329" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="B329" s="23" t="s">
+      <c r="B329" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="C329" s="23" t="s">
+      <c r="C329" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D329" s="24">
-        <v>4</v>
-      </c>
-      <c r="E329" s="25"/>
-      <c r="F329" s="25"/>
-      <c r="G329" s="25"/>
-    </row>
-    <row r="330" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D329" s="27">
+        <v>3</v>
+      </c>
+      <c r="E329" s="28"/>
+      <c r="F329" s="28"/>
+      <c r="G329" s="28"/>
+    </row>
+    <row r="330" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A330" s="23" t="s">
         <v>144</v>
       </c>
@@ -10248,11 +10836,17 @@
       <c r="D330" s="24">
         <v>5</v>
       </c>
-      <c r="E330" s="25"/>
-      <c r="F330" s="25"/>
-      <c r="G330" s="25"/>
-    </row>
-    <row r="331" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E330" s="25" t="s">
+        <v>484</v>
+      </c>
+      <c r="F330" s="25" t="s">
+        <v>485</v>
+      </c>
+      <c r="G330" s="25" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A331" s="23" t="s">
         <v>144</v>
       </c>
@@ -10265,9 +10859,15 @@
       <c r="D331" s="24">
         <v>4</v>
       </c>
-      <c r="E331" s="25"/>
-      <c r="F331" s="25"/>
-      <c r="G331" s="25"/>
+      <c r="E331" s="25" t="s">
+        <v>489</v>
+      </c>
+      <c r="F331" s="25" t="s">
+        <v>487</v>
+      </c>
+      <c r="G331" s="25" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A332" s="3" t="s">
@@ -10412,7 +11012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A342" s="23" t="s">
         <v>144</v>
       </c>
@@ -10425,9 +11025,15 @@
       <c r="D342" s="24">
         <v>4</v>
       </c>
-      <c r="E342" s="25"/>
-      <c r="F342" s="25"/>
-      <c r="G342" s="25"/>
+      <c r="E342" s="25" t="s">
+        <v>492</v>
+      </c>
+      <c r="F342" s="25" t="s">
+        <v>490</v>
+      </c>
+      <c r="G342" s="25" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="343" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">

</xml_diff>

<commit_message>
re-defined channel_narrative to channel_short_narrative so can add the long channel narratives later
</commit_message>
<xml_diff>
--- a/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
+++ b/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Downloads/rsc-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6F6CAE-0937-1541-8909-C79DDAEA4018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AD236F-4077-4B4F-AB07-554CEED0EF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="509">
   <si>
     <t>Section</t>
   </si>
@@ -1546,6 +1546,54 @@
   </si>
   <si>
     <t>high stress tolerance helps you manage unpredictable weather, scheduling conflicts, and other variables that may arise with ease</t>
+  </si>
+  <si>
+    <t>category_color</t>
+  </si>
+  <si>
+    <t>#ffc7ee</t>
+  </si>
+  <si>
+    <t>#fecaa8</t>
+  </si>
+  <si>
+    <t>#ffe7a5</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>pink</t>
+  </si>
+  <si>
+    <t>#e6eb99</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>#d7f4ff</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>#dbd9ff</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>#ffdee7</t>
+  </si>
+  <si>
+    <t>light pink</t>
+  </si>
+  <si>
+    <t>category_color_name</t>
   </si>
 </sst>
 </file>
@@ -1660,7 +1708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1731,15 +1779,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4382,80 +4421,130 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843472F9-263E-924A-9F9A-DC61CDC4480E}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="85.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="C1" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+      <c r="C2" s="14" t="s">
+        <v>494</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="C3" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>78</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="C4" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="C5" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>96</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="C6" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>101</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="C7" s="14" t="s">
+        <v>502</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>107</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>128</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -4467,8 +4556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4685398-D085-6B47-BDBF-4D7FCE78162F}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5166,7 +5255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EBBEDC-5414-B442-BDB4-EC1529FD0ACE}">
   <dimension ref="A1:G343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
+    <sheetView topLeftCell="A319" workbookViewId="0">
       <selection activeCell="F346" sqref="F346"/>
     </sheetView>
   </sheetViews>
@@ -7425,22 +7514,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="26" t="s">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B134" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="C134" s="26" t="s">
+      <c r="B134" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C134" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D134" s="27">
-        <v>5</v>
-      </c>
-      <c r="E134" s="28"/>
-      <c r="F134" s="28"/>
-      <c r="G134" s="28"/>
+      <c r="D134" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
@@ -8183,13 +8269,13 @@
       <c r="D181" s="24">
         <v>4</v>
       </c>
-      <c r="E181" s="29" t="s">
+      <c r="E181" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="F181" s="29" t="s">
+      <c r="F181" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="G181" s="29" t="s">
+      <c r="G181" s="26" t="s">
         <v>304</v>
       </c>
     </row>
@@ -8485,13 +8571,13 @@
       <c r="D200" s="24">
         <v>4</v>
       </c>
-      <c r="E200" s="29" t="s">
+      <c r="E200" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="F200" s="29" t="s">
+      <c r="F200" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="G200" s="29" t="s">
+      <c r="G200" s="26" t="s">
         <v>299</v>
       </c>
     </row>
@@ -9029,7 +9115,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" s="23" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A231" s="23" t="s">
         <v>140</v>
       </c>
@@ -10806,22 +10892,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="329" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A329" s="26" t="s">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A329" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B329" s="26" t="s">
+      <c r="B329" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C329" s="26" t="s">
+      <c r="C329" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D329" s="27">
-        <v>3</v>
-      </c>
-      <c r="E329" s="28"/>
-      <c r="F329" s="28"/>
-      <c r="G329" s="28"/>
+      <c r="D329" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="330" spans="1:7" s="23" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A330" s="23" t="s">
@@ -10897,22 +10980,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="334" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A334" s="26" t="s">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A334" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B334" s="26" t="s">
+      <c r="B334" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C334" s="26" t="s">
+      <c r="C334" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D334" s="27">
-        <v>3</v>
-      </c>
-      <c r="E334" s="28"/>
-      <c r="F334" s="28"/>
-      <c r="G334" s="28"/>
+      <c r="D334" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="s">

</xml_diff>

<commit_message>
edits to the dev code for long narratives
</commit_message>
<xml_diff>
--- a/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
+++ b/Extreme_Weighting_Scoring_Prototype_for_FormWise_REPAIRED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharon/Downloads/rsc-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AD236F-4077-4B4F-AB07-554CEED0EF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41BB53B-3964-F948-9A2B-839CE9E3B533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24820" windowHeight="21900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="527">
   <si>
     <t>Section</t>
   </si>
@@ -1594,6 +1594,60 @@
   </si>
   <si>
     <t>category_color_name</t>
+  </si>
+  <si>
+    <t>farmers_markets</t>
+  </si>
+  <si>
+    <t>subscriptions</t>
+  </si>
+  <si>
+    <t>farm_stand_farm_shop</t>
+  </si>
+  <si>
+    <t>made_to_order_designs</t>
+  </si>
+  <si>
+    <t>bulk_sales_to_the_public</t>
+  </si>
+  <si>
+    <t>wholesaling_to_florists</t>
+  </si>
+  <si>
+    <t>wholesaling_to_wholesalers</t>
+  </si>
+  <si>
+    <t>wholesaling_to_grocery_stores</t>
+  </si>
+  <si>
+    <t>wholesaling_via_a_collective</t>
+  </si>
+  <si>
+    <t>selling_as_a_stockist</t>
+  </si>
+  <si>
+    <t>selling_on_consignment</t>
+  </si>
+  <si>
+    <t>full_service_weddings</t>
+  </si>
+  <si>
+    <t>a_la_carte_weddings</t>
+  </si>
+  <si>
+    <t>community_and_corporate_events</t>
+  </si>
+  <si>
+    <t>hotel_and_restaurant_contracts</t>
+  </si>
+  <si>
+    <t>pick_your_own_events</t>
+  </si>
+  <si>
+    <t>workshops</t>
+  </si>
+  <si>
+    <t>photography_venue</t>
   </si>
 </sst>
 </file>
@@ -1603,7 +1657,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1655,6 +1709,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1708,7 +1767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1783,6 +1842,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2311,8 +2373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4556,7 +4618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4685398-D085-6B47-BDBF-4D7FCE78162F}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F20"/>
     </sheetView>
   </sheetViews>
@@ -4978,7 +5040,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4999,148 +5063,202 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="27" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="27" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="27" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="27" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="27" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="27" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="27" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="27" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="27" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="27" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="27" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" s="27" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" s="27" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" s="27" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D16" s="27" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D17" s="27" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D18" s="27" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -5255,7 +5373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EBBEDC-5414-B442-BDB4-EC1529FD0ACE}">
   <dimension ref="A1:G343"/>
   <sheetViews>
-    <sheetView topLeftCell="A319" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F346" sqref="F346"/>
     </sheetView>
   </sheetViews>

</xml_diff>